<commit_message>
Update Ann Arbor data, minor bug fixes.
</commit_message>
<xml_diff>
--- a/data/counter/export_data_domain_7992.xlsx
+++ b/data/counter/export_data_domain_7992.xlsx
@@ -69409,295 +69409,4515 @@
       <c r="A6299" s="6" t="n">
         <v>44863.5625</v>
       </c>
-      <c r="B6299" s="1"/>
-      <c r="C6299" s="1"/>
+      <c r="B6299" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6299" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="6300">
       <c r="A6300" s="6" t="n">
         <v>44863.572916666664</v>
       </c>
-      <c r="B6300" s="1"/>
-      <c r="C6300" s="1"/>
+      <c r="B6300" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C6300" s="1" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="6301">
       <c r="A6301" s="6" t="n">
         <v>44863.583333333336</v>
       </c>
-      <c r="B6301" s="1"/>
-      <c r="C6301" s="1"/>
+      <c r="B6301" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6301" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="6302">
       <c r="A6302" s="6" t="n">
         <v>44863.59375</v>
       </c>
-      <c r="B6302" s="1"/>
-      <c r="C6302" s="1"/>
+      <c r="B6302" s="1" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="C6302" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="6303">
       <c r="A6303" s="6" t="n">
         <v>44863.604166666664</v>
       </c>
-      <c r="B6303" s="1"/>
-      <c r="C6303" s="1"/>
+      <c r="B6303" s="1" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C6303" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="6304">
       <c r="A6304" s="6" t="n">
         <v>44863.614583333336</v>
       </c>
-      <c r="B6304" s="1"/>
-      <c r="C6304" s="1"/>
+      <c r="B6304" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6304" s="1" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="6305">
       <c r="A6305" s="6" t="n">
         <v>44863.625</v>
       </c>
-      <c r="B6305" s="1"/>
-      <c r="C6305" s="1"/>
+      <c r="B6305" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6305" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="6306">
       <c r="A6306" s="6" t="n">
         <v>44863.635416666664</v>
       </c>
-      <c r="B6306" s="1"/>
-      <c r="C6306" s="1"/>
+      <c r="B6306" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6306" s="1" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="6307">
       <c r="A6307" s="6" t="n">
         <v>44863.645833333336</v>
       </c>
-      <c r="B6307" s="1"/>
-      <c r="C6307" s="1"/>
+      <c r="B6307" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6307" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="6308">
       <c r="A6308" s="6" t="n">
         <v>44863.65625</v>
       </c>
-      <c r="B6308" s="1"/>
-      <c r="C6308" s="1"/>
+      <c r="B6308" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6308" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="6309">
       <c r="A6309" s="6" t="n">
         <v>44863.666666666664</v>
       </c>
-      <c r="B6309" s="1"/>
-      <c r="C6309" s="1"/>
+      <c r="B6309" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6309" s="1" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="6310">
       <c r="A6310" s="6" t="n">
         <v>44863.677083333336</v>
       </c>
-      <c r="B6310" s="1"/>
-      <c r="C6310" s="1"/>
+      <c r="B6310" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C6310" s="1" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="6311">
       <c r="A6311" s="6" t="n">
         <v>44863.6875</v>
       </c>
-      <c r="B6311" s="1"/>
-      <c r="C6311" s="1"/>
+      <c r="B6311" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6311" s="1" t="n">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="6312">
       <c r="A6312" s="6" t="n">
         <v>44863.697916666664</v>
       </c>
-      <c r="B6312" s="1"/>
-      <c r="C6312" s="1"/>
+      <c r="B6312" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6312" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="6313">
       <c r="A6313" s="6" t="n">
         <v>44863.708333333336</v>
       </c>
-      <c r="B6313" s="1"/>
-      <c r="C6313" s="1"/>
+      <c r="B6313" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C6313" s="1" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="6314">
       <c r="A6314" s="6" t="n">
         <v>44863.71875</v>
       </c>
-      <c r="B6314" s="1"/>
-      <c r="C6314" s="1"/>
+      <c r="B6314" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6314" s="1" t="n">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="6315">
       <c r="A6315" s="6" t="n">
         <v>44863.729166666664</v>
       </c>
-      <c r="B6315" s="1"/>
-      <c r="C6315" s="1"/>
+      <c r="B6315" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C6315" s="1" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="6316">
       <c r="A6316" s="6" t="n">
         <v>44863.739583333336</v>
       </c>
-      <c r="B6316" s="1"/>
-      <c r="C6316" s="1"/>
+      <c r="B6316" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6316" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="6317">
       <c r="A6317" s="6" t="n">
         <v>44863.75</v>
       </c>
-      <c r="B6317" s="1"/>
-      <c r="C6317" s="1"/>
+      <c r="B6317" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6317" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="6318">
       <c r="A6318" s="6" t="n">
         <v>44863.760416666664</v>
       </c>
-      <c r="B6318" s="1"/>
-      <c r="C6318" s="1"/>
+      <c r="B6318" s="1" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="C6318" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="6319">
       <c r="A6319" s="6" t="n">
         <v>44863.770833333336</v>
       </c>
-      <c r="B6319" s="1"/>
-      <c r="C6319" s="1"/>
+      <c r="B6319" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6319" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="6320">
       <c r="A6320" s="6" t="n">
         <v>44863.78125</v>
       </c>
-      <c r="B6320" s="1"/>
-      <c r="C6320" s="1"/>
+      <c r="B6320" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C6320" s="1" t="n">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="6321">
       <c r="A6321" s="6" t="n">
         <v>44863.791666666664</v>
       </c>
-      <c r="B6321" s="1"/>
-      <c r="C6321" s="1"/>
+      <c r="B6321" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C6321" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="6322">
       <c r="A6322" s="6" t="n">
         <v>44863.802083333336</v>
       </c>
-      <c r="B6322" s="1"/>
-      <c r="C6322" s="1"/>
+      <c r="B6322" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6322" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="6323">
       <c r="A6323" s="6" t="n">
         <v>44863.8125</v>
       </c>
-      <c r="B6323" s="1"/>
-      <c r="C6323" s="1"/>
+      <c r="B6323" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C6323" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="6324">
       <c r="A6324" s="6" t="n">
         <v>44863.822916666664</v>
       </c>
-      <c r="B6324" s="1"/>
-      <c r="C6324" s="1"/>
+      <c r="B6324" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6324" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="6325">
       <c r="A6325" s="6" t="n">
         <v>44863.833333333336</v>
       </c>
-      <c r="B6325" s="1"/>
-      <c r="C6325" s="1"/>
+      <c r="B6325" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6325" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="6326">
       <c r="A6326" s="6" t="n">
         <v>44863.84375</v>
       </c>
-      <c r="B6326" s="1"/>
-      <c r="C6326" s="1"/>
+      <c r="B6326" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6326" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="6327">
       <c r="A6327" s="6" t="n">
         <v>44863.854166666664</v>
       </c>
-      <c r="B6327" s="1"/>
-      <c r="C6327" s="1"/>
+      <c r="B6327" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6327" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="6328">
       <c r="A6328" s="6" t="n">
         <v>44863.864583333336</v>
       </c>
-      <c r="B6328" s="1"/>
-      <c r="C6328" s="1"/>
+      <c r="B6328" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6328" s="1" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="6329">
       <c r="A6329" s="6" t="n">
         <v>44863.875</v>
       </c>
-      <c r="B6329" s="1"/>
-      <c r="C6329" s="1"/>
+      <c r="B6329" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6329" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="6330">
       <c r="A6330" s="6" t="n">
         <v>44863.885416666664</v>
       </c>
-      <c r="B6330" s="1"/>
-      <c r="C6330" s="1"/>
+      <c r="B6330" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6330" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="6331">
       <c r="A6331" s="6" t="n">
         <v>44863.895833333336</v>
       </c>
-      <c r="B6331" s="1"/>
-      <c r="C6331" s="1"/>
+      <c r="B6331" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6331" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="6332">
       <c r="A6332" s="6" t="n">
         <v>44863.90625</v>
       </c>
-      <c r="B6332" s="1"/>
-      <c r="C6332" s="1"/>
+      <c r="B6332" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6332" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="6333">
       <c r="A6333" s="6" t="n">
         <v>44863.916666666664</v>
       </c>
-      <c r="B6333" s="1"/>
-      <c r="C6333" s="1"/>
+      <c r="B6333" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6333" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="6334">
       <c r="A6334" s="6" t="n">
         <v>44863.927083333336</v>
       </c>
-      <c r="B6334" s="1"/>
-      <c r="C6334" s="1"/>
+      <c r="B6334" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6334" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="6335">
       <c r="A6335" s="6" t="n">
         <v>44863.9375</v>
       </c>
-      <c r="B6335" s="1"/>
-      <c r="C6335" s="1"/>
+      <c r="B6335" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6335" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="6336">
       <c r="A6336" s="6" t="n">
         <v>44863.947916666664</v>
       </c>
-      <c r="B6336" s="1"/>
-      <c r="C6336" s="1"/>
+      <c r="B6336" s="1" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="C6336" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="6337">
       <c r="A6337" s="6" t="n">
         <v>44863.958333333336</v>
       </c>
-      <c r="B6337" s="1"/>
-      <c r="C6337" s="1"/>
+      <c r="B6337" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6337" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="6338">
       <c r="A6338" s="6" t="n">
         <v>44863.96875</v>
       </c>
-      <c r="B6338" s="1"/>
-      <c r="C6338" s="1"/>
+      <c r="B6338" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C6338" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="6339">
       <c r="A6339" s="6" t="n">
         <v>44863.979166666664</v>
       </c>
-      <c r="B6339" s="1"/>
-      <c r="C6339" s="1"/>
+      <c r="B6339" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6339" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="6340">
       <c r="A6340" s="6" t="n">
         <v>44863.989583333336</v>
       </c>
-      <c r="B6340" s="1"/>
-      <c r="C6340" s="1"/>
+      <c r="B6340" s="1" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C6340" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6341">
+      <c r="A6341" s="6" t="n">
+        <v>44864.0</v>
+      </c>
+      <c r="B6341" s="1" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C6341" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6342">
+      <c r="A6342" s="6" t="n">
+        <v>44864.010416666664</v>
+      </c>
+      <c r="B6342" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6342" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6343">
+      <c r="A6343" s="6" t="n">
+        <v>44864.020833333336</v>
+      </c>
+      <c r="B6343" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6343" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6344">
+      <c r="A6344" s="6" t="n">
+        <v>44864.03125</v>
+      </c>
+      <c r="B6344" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6344" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6345">
+      <c r="A6345" s="6" t="n">
+        <v>44864.041666666664</v>
+      </c>
+      <c r="B6345" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6345" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6346">
+      <c r="A6346" s="6" t="n">
+        <v>44864.052083333336</v>
+      </c>
+      <c r="B6346" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6346" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6347">
+      <c r="A6347" s="6" t="n">
+        <v>44864.0625</v>
+      </c>
+      <c r="B6347" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6347" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6348">
+      <c r="A6348" s="6" t="n">
+        <v>44864.072916666664</v>
+      </c>
+      <c r="B6348" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6348" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6349">
+      <c r="A6349" s="6" t="n">
+        <v>44864.083333333336</v>
+      </c>
+      <c r="B6349" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6349" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6350">
+      <c r="A6350" s="6" t="n">
+        <v>44864.09375</v>
+      </c>
+      <c r="B6350" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6350" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6351">
+      <c r="A6351" s="6" t="n">
+        <v>44864.104166666664</v>
+      </c>
+      <c r="B6351" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6351" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6352">
+      <c r="A6352" s="6" t="n">
+        <v>44864.114583333336</v>
+      </c>
+      <c r="B6352" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6352" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6353">
+      <c r="A6353" s="6" t="n">
+        <v>44864.125</v>
+      </c>
+      <c r="B6353" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6353" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6354">
+      <c r="A6354" s="6" t="n">
+        <v>44864.135416666664</v>
+      </c>
+      <c r="B6354" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6354" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6355">
+      <c r="A6355" s="6" t="n">
+        <v>44864.145833333336</v>
+      </c>
+      <c r="B6355" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6355" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6356">
+      <c r="A6356" s="6" t="n">
+        <v>44864.15625</v>
+      </c>
+      <c r="B6356" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6356" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6357">
+      <c r="A6357" s="6" t="n">
+        <v>44864.166666666664</v>
+      </c>
+      <c r="B6357" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6357" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6358">
+      <c r="A6358" s="6" t="n">
+        <v>44864.177083333336</v>
+      </c>
+      <c r="B6358" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6358" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6359">
+      <c r="A6359" s="6" t="n">
+        <v>44864.1875</v>
+      </c>
+      <c r="B6359" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6359" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6360">
+      <c r="A6360" s="6" t="n">
+        <v>44864.197916666664</v>
+      </c>
+      <c r="B6360" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6360" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6361">
+      <c r="A6361" s="6" t="n">
+        <v>44864.208333333336</v>
+      </c>
+      <c r="B6361" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6361" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6362">
+      <c r="A6362" s="6" t="n">
+        <v>44864.21875</v>
+      </c>
+      <c r="B6362" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6362" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6363">
+      <c r="A6363" s="6" t="n">
+        <v>44864.229166666664</v>
+      </c>
+      <c r="B6363" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6363" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6364">
+      <c r="A6364" s="6" t="n">
+        <v>44864.239583333336</v>
+      </c>
+      <c r="B6364" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6364" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6365">
+      <c r="A6365" s="6" t="n">
+        <v>44864.25</v>
+      </c>
+      <c r="B6365" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6365" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6366">
+      <c r="A6366" s="6" t="n">
+        <v>44864.260416666664</v>
+      </c>
+      <c r="B6366" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6366" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6367">
+      <c r="A6367" s="6" t="n">
+        <v>44864.270833333336</v>
+      </c>
+      <c r="B6367" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6367" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6368">
+      <c r="A6368" s="6" t="n">
+        <v>44864.28125</v>
+      </c>
+      <c r="B6368" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6368" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6369">
+      <c r="A6369" s="6" t="n">
+        <v>44864.291666666664</v>
+      </c>
+      <c r="B6369" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6369" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6370">
+      <c r="A6370" s="6" t="n">
+        <v>44864.302083333336</v>
+      </c>
+      <c r="B6370" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6370" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6371">
+      <c r="A6371" s="6" t="n">
+        <v>44864.3125</v>
+      </c>
+      <c r="B6371" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6371" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6372">
+      <c r="A6372" s="6" t="n">
+        <v>44864.322916666664</v>
+      </c>
+      <c r="B6372" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6372" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6373">
+      <c r="A6373" s="6" t="n">
+        <v>44864.333333333336</v>
+      </c>
+      <c r="B6373" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6373" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6374">
+      <c r="A6374" s="6" t="n">
+        <v>44864.34375</v>
+      </c>
+      <c r="B6374" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6374" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6375">
+      <c r="A6375" s="6" t="n">
+        <v>44864.354166666664</v>
+      </c>
+      <c r="B6375" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6375" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6376">
+      <c r="A6376" s="6" t="n">
+        <v>44864.364583333336</v>
+      </c>
+      <c r="B6376" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6376" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6377">
+      <c r="A6377" s="6" t="n">
+        <v>44864.375</v>
+      </c>
+      <c r="B6377" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6377" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6378">
+      <c r="A6378" s="6" t="n">
+        <v>44864.385416666664</v>
+      </c>
+      <c r="B6378" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6378" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6379">
+      <c r="A6379" s="6" t="n">
+        <v>44864.395833333336</v>
+      </c>
+      <c r="B6379" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6379" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6380">
+      <c r="A6380" s="6" t="n">
+        <v>44864.40625</v>
+      </c>
+      <c r="B6380" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6380" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6381">
+      <c r="A6381" s="6" t="n">
+        <v>44864.416666666664</v>
+      </c>
+      <c r="B6381" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6381" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6382">
+      <c r="A6382" s="6" t="n">
+        <v>44864.427083333336</v>
+      </c>
+      <c r="B6382" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6382" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6383">
+      <c r="A6383" s="6" t="n">
+        <v>44864.4375</v>
+      </c>
+      <c r="B6383" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6383" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6384">
+      <c r="A6384" s="6" t="n">
+        <v>44864.447916666664</v>
+      </c>
+      <c r="B6384" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6384" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6385">
+      <c r="A6385" s="6" t="n">
+        <v>44864.458333333336</v>
+      </c>
+      <c r="B6385" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6385" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6386">
+      <c r="A6386" s="6" t="n">
+        <v>44864.46875</v>
+      </c>
+      <c r="B6386" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6386" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6387">
+      <c r="A6387" s="6" t="n">
+        <v>44864.479166666664</v>
+      </c>
+      <c r="B6387" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6387" s="1" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="6388">
+      <c r="A6388" s="6" t="n">
+        <v>44864.489583333336</v>
+      </c>
+      <c r="B6388" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6388" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6389">
+      <c r="A6389" s="6" t="n">
+        <v>44864.5</v>
+      </c>
+      <c r="B6389" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6389" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6390">
+      <c r="A6390" s="6" t="n">
+        <v>44864.510416666664</v>
+      </c>
+      <c r="B6390" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6390" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6391">
+      <c r="A6391" s="6" t="n">
+        <v>44864.520833333336</v>
+      </c>
+      <c r="B6391" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6391" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6392">
+      <c r="A6392" s="6" t="n">
+        <v>44864.53125</v>
+      </c>
+      <c r="B6392" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6392" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6393">
+      <c r="A6393" s="6" t="n">
+        <v>44864.541666666664</v>
+      </c>
+      <c r="B6393" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6393" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6394">
+      <c r="A6394" s="6" t="n">
+        <v>44864.552083333336</v>
+      </c>
+      <c r="B6394" s="1" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C6394" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6395">
+      <c r="A6395" s="6" t="n">
+        <v>44864.5625</v>
+      </c>
+      <c r="B6395" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C6395" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="6396">
+      <c r="A6396" s="6" t="n">
+        <v>44864.572916666664</v>
+      </c>
+      <c r="B6396" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6396" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6397">
+      <c r="A6397" s="6" t="n">
+        <v>44864.583333333336</v>
+      </c>
+      <c r="B6397" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6397" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6398">
+      <c r="A6398" s="6" t="n">
+        <v>44864.59375</v>
+      </c>
+      <c r="B6398" s="1" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C6398" s="1" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="6399">
+      <c r="A6399" s="6" t="n">
+        <v>44864.604166666664</v>
+      </c>
+      <c r="B6399" s="1" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C6399" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6400">
+      <c r="A6400" s="6" t="n">
+        <v>44864.614583333336</v>
+      </c>
+      <c r="B6400" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6400" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6401">
+      <c r="A6401" s="6" t="n">
+        <v>44864.625</v>
+      </c>
+      <c r="B6401" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6401" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="6402">
+      <c r="A6402" s="6" t="n">
+        <v>44864.635416666664</v>
+      </c>
+      <c r="B6402" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6402" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6403">
+      <c r="A6403" s="6" t="n">
+        <v>44864.645833333336</v>
+      </c>
+      <c r="B6403" s="1" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C6403" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6404">
+      <c r="A6404" s="6" t="n">
+        <v>44864.65625</v>
+      </c>
+      <c r="B6404" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C6404" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6405">
+      <c r="A6405" s="6" t="n">
+        <v>44864.666666666664</v>
+      </c>
+      <c r="B6405" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6405" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6406">
+      <c r="A6406" s="6" t="n">
+        <v>44864.677083333336</v>
+      </c>
+      <c r="B6406" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6406" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6407">
+      <c r="A6407" s="6" t="n">
+        <v>44864.6875</v>
+      </c>
+      <c r="B6407" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C6407" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="6408">
+      <c r="A6408" s="6" t="n">
+        <v>44864.697916666664</v>
+      </c>
+      <c r="B6408" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6408" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6409">
+      <c r="A6409" s="6" t="n">
+        <v>44864.708333333336</v>
+      </c>
+      <c r="B6409" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C6409" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6410">
+      <c r="A6410" s="6" t="n">
+        <v>44864.71875</v>
+      </c>
+      <c r="B6410" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6410" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6411">
+      <c r="A6411" s="6" t="n">
+        <v>44864.729166666664</v>
+      </c>
+      <c r="B6411" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C6411" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6412">
+      <c r="A6412" s="6" t="n">
+        <v>44864.739583333336</v>
+      </c>
+      <c r="B6412" s="1" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C6412" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6413">
+      <c r="A6413" s="6" t="n">
+        <v>44864.75</v>
+      </c>
+      <c r="B6413" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C6413" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6414">
+      <c r="A6414" s="6" t="n">
+        <v>44864.760416666664</v>
+      </c>
+      <c r="B6414" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6414" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6415">
+      <c r="A6415" s="6" t="n">
+        <v>44864.770833333336</v>
+      </c>
+      <c r="B6415" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6415" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6416">
+      <c r="A6416" s="6" t="n">
+        <v>44864.78125</v>
+      </c>
+      <c r="B6416" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6416" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6417">
+      <c r="A6417" s="6" t="n">
+        <v>44864.791666666664</v>
+      </c>
+      <c r="B6417" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6417" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6418">
+      <c r="A6418" s="6" t="n">
+        <v>44864.802083333336</v>
+      </c>
+      <c r="B6418" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6418" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6419">
+      <c r="A6419" s="6" t="n">
+        <v>44864.8125</v>
+      </c>
+      <c r="B6419" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6419" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6420">
+      <c r="A6420" s="6" t="n">
+        <v>44864.822916666664</v>
+      </c>
+      <c r="B6420" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6420" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6421">
+      <c r="A6421" s="6" t="n">
+        <v>44864.833333333336</v>
+      </c>
+      <c r="B6421" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6421" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6422">
+      <c r="A6422" s="6" t="n">
+        <v>44864.84375</v>
+      </c>
+      <c r="B6422" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6422" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6423">
+      <c r="A6423" s="6" t="n">
+        <v>44864.854166666664</v>
+      </c>
+      <c r="B6423" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6423" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6424">
+      <c r="A6424" s="6" t="n">
+        <v>44864.864583333336</v>
+      </c>
+      <c r="B6424" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6424" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6425">
+      <c r="A6425" s="6" t="n">
+        <v>44864.875</v>
+      </c>
+      <c r="B6425" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6425" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6426">
+      <c r="A6426" s="6" t="n">
+        <v>44864.885416666664</v>
+      </c>
+      <c r="B6426" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6426" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6427">
+      <c r="A6427" s="6" t="n">
+        <v>44864.895833333336</v>
+      </c>
+      <c r="B6427" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6427" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6428">
+      <c r="A6428" s="6" t="n">
+        <v>44864.90625</v>
+      </c>
+      <c r="B6428" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6428" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6429">
+      <c r="A6429" s="6" t="n">
+        <v>44864.916666666664</v>
+      </c>
+      <c r="B6429" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6429" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6430">
+      <c r="A6430" s="6" t="n">
+        <v>44864.927083333336</v>
+      </c>
+      <c r="B6430" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6430" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6431">
+      <c r="A6431" s="6" t="n">
+        <v>44864.9375</v>
+      </c>
+      <c r="B6431" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6431" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6432">
+      <c r="A6432" s="6" t="n">
+        <v>44864.947916666664</v>
+      </c>
+      <c r="B6432" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6432" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6433">
+      <c r="A6433" s="6" t="n">
+        <v>44864.958333333336</v>
+      </c>
+      <c r="B6433" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6433" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6434">
+      <c r="A6434" s="6" t="n">
+        <v>44864.96875</v>
+      </c>
+      <c r="B6434" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6434" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6435">
+      <c r="A6435" s="6" t="n">
+        <v>44864.979166666664</v>
+      </c>
+      <c r="B6435" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6435" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6436">
+      <c r="A6436" s="6" t="n">
+        <v>44864.989583333336</v>
+      </c>
+      <c r="B6436" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6436" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6437">
+      <c r="A6437" s="6" t="n">
+        <v>44865.0</v>
+      </c>
+      <c r="B6437" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6437" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6438">
+      <c r="A6438" s="6" t="n">
+        <v>44865.010416666664</v>
+      </c>
+      <c r="B6438" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6438" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6439">
+      <c r="A6439" s="6" t="n">
+        <v>44865.020833333336</v>
+      </c>
+      <c r="B6439" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6439" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6440">
+      <c r="A6440" s="6" t="n">
+        <v>44865.03125</v>
+      </c>
+      <c r="B6440" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6440" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6441">
+      <c r="A6441" s="6" t="n">
+        <v>44865.041666666664</v>
+      </c>
+      <c r="B6441" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6441" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6442">
+      <c r="A6442" s="6" t="n">
+        <v>44865.052083333336</v>
+      </c>
+      <c r="B6442" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6442" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6443">
+      <c r="A6443" s="6" t="n">
+        <v>44865.0625</v>
+      </c>
+      <c r="B6443" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6443" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6444">
+      <c r="A6444" s="6" t="n">
+        <v>44865.072916666664</v>
+      </c>
+      <c r="B6444" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6444" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6445">
+      <c r="A6445" s="6" t="n">
+        <v>44865.083333333336</v>
+      </c>
+      <c r="B6445" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6445" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6446">
+      <c r="A6446" s="6" t="n">
+        <v>44865.09375</v>
+      </c>
+      <c r="B6446" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6446" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6447">
+      <c r="A6447" s="6" t="n">
+        <v>44865.104166666664</v>
+      </c>
+      <c r="B6447" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6447" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6448">
+      <c r="A6448" s="6" t="n">
+        <v>44865.114583333336</v>
+      </c>
+      <c r="B6448" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6448" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6449">
+      <c r="A6449" s="6" t="n">
+        <v>44865.125</v>
+      </c>
+      <c r="B6449" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6449" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6450">
+      <c r="A6450" s="6" t="n">
+        <v>44865.135416666664</v>
+      </c>
+      <c r="B6450" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6450" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6451">
+      <c r="A6451" s="6" t="n">
+        <v>44865.145833333336</v>
+      </c>
+      <c r="B6451" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6451" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6452">
+      <c r="A6452" s="6" t="n">
+        <v>44865.15625</v>
+      </c>
+      <c r="B6452" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6452" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6453">
+      <c r="A6453" s="6" t="n">
+        <v>44865.166666666664</v>
+      </c>
+      <c r="B6453" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6453" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6454">
+      <c r="A6454" s="6" t="n">
+        <v>44865.177083333336</v>
+      </c>
+      <c r="B6454" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6454" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6455">
+      <c r="A6455" s="6" t="n">
+        <v>44865.1875</v>
+      </c>
+      <c r="B6455" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6455" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6456">
+      <c r="A6456" s="6" t="n">
+        <v>44865.197916666664</v>
+      </c>
+      <c r="B6456" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6456" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6457">
+      <c r="A6457" s="6" t="n">
+        <v>44865.208333333336</v>
+      </c>
+      <c r="B6457" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6457" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6458">
+      <c r="A6458" s="6" t="n">
+        <v>44865.21875</v>
+      </c>
+      <c r="B6458" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6458" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6459">
+      <c r="A6459" s="6" t="n">
+        <v>44865.229166666664</v>
+      </c>
+      <c r="B6459" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6459" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6460">
+      <c r="A6460" s="6" t="n">
+        <v>44865.239583333336</v>
+      </c>
+      <c r="B6460" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6460" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6461">
+      <c r="A6461" s="6" t="n">
+        <v>44865.25</v>
+      </c>
+      <c r="B6461" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6461" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6462">
+      <c r="A6462" s="6" t="n">
+        <v>44865.260416666664</v>
+      </c>
+      <c r="B6462" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6462" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6463">
+      <c r="A6463" s="6" t="n">
+        <v>44865.270833333336</v>
+      </c>
+      <c r="B6463" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6463" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6464">
+      <c r="A6464" s="6" t="n">
+        <v>44865.28125</v>
+      </c>
+      <c r="B6464" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6464" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6465">
+      <c r="A6465" s="6" t="n">
+        <v>44865.291666666664</v>
+      </c>
+      <c r="B6465" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6465" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6466">
+      <c r="A6466" s="6" t="n">
+        <v>44865.302083333336</v>
+      </c>
+      <c r="B6466" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6466" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6467">
+      <c r="A6467" s="6" t="n">
+        <v>44865.3125</v>
+      </c>
+      <c r="B6467" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6467" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6468">
+      <c r="A6468" s="6" t="n">
+        <v>44865.322916666664</v>
+      </c>
+      <c r="B6468" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C6468" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6469">
+      <c r="A6469" s="6" t="n">
+        <v>44865.333333333336</v>
+      </c>
+      <c r="B6469" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6469" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6470">
+      <c r="A6470" s="6" t="n">
+        <v>44865.34375</v>
+      </c>
+      <c r="B6470" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6470" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="6471">
+      <c r="A6471" s="6" t="n">
+        <v>44865.354166666664</v>
+      </c>
+      <c r="B6471" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6471" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6472">
+      <c r="A6472" s="6" t="n">
+        <v>44865.364583333336</v>
+      </c>
+      <c r="B6472" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6472" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6473">
+      <c r="A6473" s="6" t="n">
+        <v>44865.375</v>
+      </c>
+      <c r="B6473" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6473" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6474">
+      <c r="A6474" s="6" t="n">
+        <v>44865.385416666664</v>
+      </c>
+      <c r="B6474" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6474" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6475">
+      <c r="A6475" s="6" t="n">
+        <v>44865.395833333336</v>
+      </c>
+      <c r="B6475" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6475" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6476">
+      <c r="A6476" s="6" t="n">
+        <v>44865.40625</v>
+      </c>
+      <c r="B6476" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6476" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6477">
+      <c r="A6477" s="6" t="n">
+        <v>44865.416666666664</v>
+      </c>
+      <c r="B6477" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6477" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6478">
+      <c r="A6478" s="6" t="n">
+        <v>44865.427083333336</v>
+      </c>
+      <c r="B6478" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6478" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6479">
+      <c r="A6479" s="6" t="n">
+        <v>44865.4375</v>
+      </c>
+      <c r="B6479" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6479" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6480">
+      <c r="A6480" s="6" t="n">
+        <v>44865.447916666664</v>
+      </c>
+      <c r="B6480" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6480" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6481">
+      <c r="A6481" s="6" t="n">
+        <v>44865.458333333336</v>
+      </c>
+      <c r="B6481" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6481" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6482">
+      <c r="A6482" s="6" t="n">
+        <v>44865.46875</v>
+      </c>
+      <c r="B6482" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6482" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6483">
+      <c r="A6483" s="6" t="n">
+        <v>44865.479166666664</v>
+      </c>
+      <c r="B6483" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6483" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6484">
+      <c r="A6484" s="6" t="n">
+        <v>44865.489583333336</v>
+      </c>
+      <c r="B6484" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6484" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="6485">
+      <c r="A6485" s="6" t="n">
+        <v>44865.5</v>
+      </c>
+      <c r="B6485" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6485" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6486">
+      <c r="A6486" s="6" t="n">
+        <v>44865.510416666664</v>
+      </c>
+      <c r="B6486" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6486" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6487">
+      <c r="A6487" s="6" t="n">
+        <v>44865.520833333336</v>
+      </c>
+      <c r="B6487" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6487" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6488">
+      <c r="A6488" s="6" t="n">
+        <v>44865.53125</v>
+      </c>
+      <c r="B6488" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6488" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6489">
+      <c r="A6489" s="6" t="n">
+        <v>44865.541666666664</v>
+      </c>
+      <c r="B6489" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6489" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6490">
+      <c r="A6490" s="6" t="n">
+        <v>44865.552083333336</v>
+      </c>
+      <c r="B6490" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6490" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6491">
+      <c r="A6491" s="6" t="n">
+        <v>44865.5625</v>
+      </c>
+      <c r="B6491" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6491" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6492">
+      <c r="A6492" s="6" t="n">
+        <v>44865.572916666664</v>
+      </c>
+      <c r="B6492" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6492" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6493">
+      <c r="A6493" s="6" t="n">
+        <v>44865.583333333336</v>
+      </c>
+      <c r="B6493" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6493" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6494">
+      <c r="A6494" s="6" t="n">
+        <v>44865.59375</v>
+      </c>
+      <c r="B6494" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6494" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6495">
+      <c r="A6495" s="6" t="n">
+        <v>44865.604166666664</v>
+      </c>
+      <c r="B6495" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C6495" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6496">
+      <c r="A6496" s="6" t="n">
+        <v>44865.614583333336</v>
+      </c>
+      <c r="B6496" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6496" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6497">
+      <c r="A6497" s="6" t="n">
+        <v>44865.625</v>
+      </c>
+      <c r="B6497" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6497" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6498">
+      <c r="A6498" s="6" t="n">
+        <v>44865.635416666664</v>
+      </c>
+      <c r="B6498" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6498" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6499">
+      <c r="A6499" s="6" t="n">
+        <v>44865.645833333336</v>
+      </c>
+      <c r="B6499" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6499" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6500">
+      <c r="A6500" s="6" t="n">
+        <v>44865.65625</v>
+      </c>
+      <c r="B6500" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6500" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6501">
+      <c r="A6501" s="6" t="n">
+        <v>44865.666666666664</v>
+      </c>
+      <c r="B6501" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C6501" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6502">
+      <c r="A6502" s="6" t="n">
+        <v>44865.677083333336</v>
+      </c>
+      <c r="B6502" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6502" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6503">
+      <c r="A6503" s="6" t="n">
+        <v>44865.6875</v>
+      </c>
+      <c r="B6503" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6503" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6504">
+      <c r="A6504" s="6" t="n">
+        <v>44865.697916666664</v>
+      </c>
+      <c r="B6504" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6504" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6505">
+      <c r="A6505" s="6" t="n">
+        <v>44865.708333333336</v>
+      </c>
+      <c r="B6505" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6505" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="6506">
+      <c r="A6506" s="6" t="n">
+        <v>44865.71875</v>
+      </c>
+      <c r="B6506" s="1" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="C6506" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6507">
+      <c r="A6507" s="6" t="n">
+        <v>44865.729166666664</v>
+      </c>
+      <c r="B6507" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6507" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6508">
+      <c r="A6508" s="6" t="n">
+        <v>44865.739583333336</v>
+      </c>
+      <c r="B6508" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6508" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6509">
+      <c r="A6509" s="6" t="n">
+        <v>44865.75</v>
+      </c>
+      <c r="B6509" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6509" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6510">
+      <c r="A6510" s="6" t="n">
+        <v>44865.760416666664</v>
+      </c>
+      <c r="B6510" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6510" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6511">
+      <c r="A6511" s="6" t="n">
+        <v>44865.770833333336</v>
+      </c>
+      <c r="B6511" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6511" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6512">
+      <c r="A6512" s="6" t="n">
+        <v>44865.78125</v>
+      </c>
+      <c r="B6512" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6512" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6513">
+      <c r="A6513" s="6" t="n">
+        <v>44865.791666666664</v>
+      </c>
+      <c r="B6513" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6513" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6514">
+      <c r="A6514" s="6" t="n">
+        <v>44865.802083333336</v>
+      </c>
+      <c r="B6514" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6514" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="6515">
+      <c r="A6515" s="6" t="n">
+        <v>44865.8125</v>
+      </c>
+      <c r="B6515" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6515" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6516">
+      <c r="A6516" s="6" t="n">
+        <v>44865.822916666664</v>
+      </c>
+      <c r="B6516" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6516" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6517">
+      <c r="A6517" s="6" t="n">
+        <v>44865.833333333336</v>
+      </c>
+      <c r="B6517" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6517" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6518">
+      <c r="A6518" s="6" t="n">
+        <v>44865.84375</v>
+      </c>
+      <c r="B6518" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6518" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6519">
+      <c r="A6519" s="6" t="n">
+        <v>44865.854166666664</v>
+      </c>
+      <c r="B6519" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6519" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6520">
+      <c r="A6520" s="6" t="n">
+        <v>44865.864583333336</v>
+      </c>
+      <c r="B6520" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6520" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6521">
+      <c r="A6521" s="6" t="n">
+        <v>44865.875</v>
+      </c>
+      <c r="B6521" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6521" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6522">
+      <c r="A6522" s="6" t="n">
+        <v>44865.885416666664</v>
+      </c>
+      <c r="B6522" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6522" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6523">
+      <c r="A6523" s="6" t="n">
+        <v>44865.895833333336</v>
+      </c>
+      <c r="B6523" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6523" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6524">
+      <c r="A6524" s="6" t="n">
+        <v>44865.90625</v>
+      </c>
+      <c r="B6524" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6524" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6525">
+      <c r="A6525" s="6" t="n">
+        <v>44865.916666666664</v>
+      </c>
+      <c r="B6525" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6525" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6526">
+      <c r="A6526" s="6" t="n">
+        <v>44865.927083333336</v>
+      </c>
+      <c r="B6526" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6526" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6527">
+      <c r="A6527" s="6" t="n">
+        <v>44865.9375</v>
+      </c>
+      <c r="B6527" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6527" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6528">
+      <c r="A6528" s="6" t="n">
+        <v>44865.947916666664</v>
+      </c>
+      <c r="B6528" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6528" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6529">
+      <c r="A6529" s="6" t="n">
+        <v>44865.958333333336</v>
+      </c>
+      <c r="B6529" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6529" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6530">
+      <c r="A6530" s="6" t="n">
+        <v>44865.96875</v>
+      </c>
+      <c r="B6530" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6530" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6531">
+      <c r="A6531" s="6" t="n">
+        <v>44865.979166666664</v>
+      </c>
+      <c r="B6531" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6531" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6532">
+      <c r="A6532" s="6" t="n">
+        <v>44865.989583333336</v>
+      </c>
+      <c r="B6532" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6532" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6533">
+      <c r="A6533" s="6" t="n">
+        <v>44866.0</v>
+      </c>
+      <c r="B6533" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6533" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6534">
+      <c r="A6534" s="6" t="n">
+        <v>44866.010416666664</v>
+      </c>
+      <c r="B6534" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6534" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6535">
+      <c r="A6535" s="6" t="n">
+        <v>44866.020833333336</v>
+      </c>
+      <c r="B6535" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6535" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6536">
+      <c r="A6536" s="6" t="n">
+        <v>44866.03125</v>
+      </c>
+      <c r="B6536" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6536" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6537">
+      <c r="A6537" s="6" t="n">
+        <v>44866.041666666664</v>
+      </c>
+      <c r="B6537" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6537" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6538">
+      <c r="A6538" s="6" t="n">
+        <v>44866.052083333336</v>
+      </c>
+      <c r="B6538" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6538" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6539">
+      <c r="A6539" s="6" t="n">
+        <v>44866.0625</v>
+      </c>
+      <c r="B6539" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6539" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6540">
+      <c r="A6540" s="6" t="n">
+        <v>44866.072916666664</v>
+      </c>
+      <c r="B6540" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6540" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6541">
+      <c r="A6541" s="6" t="n">
+        <v>44866.083333333336</v>
+      </c>
+      <c r="B6541" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6541" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6542">
+      <c r="A6542" s="6" t="n">
+        <v>44866.09375</v>
+      </c>
+      <c r="B6542" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6542" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6543">
+      <c r="A6543" s="6" t="n">
+        <v>44866.104166666664</v>
+      </c>
+      <c r="B6543" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6543" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6544">
+      <c r="A6544" s="6" t="n">
+        <v>44866.114583333336</v>
+      </c>
+      <c r="B6544" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6544" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6545">
+      <c r="A6545" s="6" t="n">
+        <v>44866.125</v>
+      </c>
+      <c r="B6545" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6545" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6546">
+      <c r="A6546" s="6" t="n">
+        <v>44866.135416666664</v>
+      </c>
+      <c r="B6546" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6546" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6547">
+      <c r="A6547" s="6" t="n">
+        <v>44866.145833333336</v>
+      </c>
+      <c r="B6547" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6547" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6548">
+      <c r="A6548" s="6" t="n">
+        <v>44866.15625</v>
+      </c>
+      <c r="B6548" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6548" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6549">
+      <c r="A6549" s="6" t="n">
+        <v>44866.166666666664</v>
+      </c>
+      <c r="B6549" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6549" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6550">
+      <c r="A6550" s="6" t="n">
+        <v>44866.177083333336</v>
+      </c>
+      <c r="B6550" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6550" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6551">
+      <c r="A6551" s="6" t="n">
+        <v>44866.1875</v>
+      </c>
+      <c r="B6551" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6551" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6552">
+      <c r="A6552" s="6" t="n">
+        <v>44866.197916666664</v>
+      </c>
+      <c r="B6552" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6552" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6553">
+      <c r="A6553" s="6" t="n">
+        <v>44866.208333333336</v>
+      </c>
+      <c r="B6553" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6553" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6554">
+      <c r="A6554" s="6" t="n">
+        <v>44866.21875</v>
+      </c>
+      <c r="B6554" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6554" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6555">
+      <c r="A6555" s="6" t="n">
+        <v>44866.229166666664</v>
+      </c>
+      <c r="B6555" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6555" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6556">
+      <c r="A6556" s="6" t="n">
+        <v>44866.239583333336</v>
+      </c>
+      <c r="B6556" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6556" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6557">
+      <c r="A6557" s="6" t="n">
+        <v>44866.25</v>
+      </c>
+      <c r="B6557" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6557" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6558">
+      <c r="A6558" s="6" t="n">
+        <v>44866.260416666664</v>
+      </c>
+      <c r="B6558" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6558" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6559">
+      <c r="A6559" s="6" t="n">
+        <v>44866.270833333336</v>
+      </c>
+      <c r="B6559" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6559" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6560">
+      <c r="A6560" s="6" t="n">
+        <v>44866.28125</v>
+      </c>
+      <c r="B6560" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6560" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6561">
+      <c r="A6561" s="6" t="n">
+        <v>44866.291666666664</v>
+      </c>
+      <c r="B6561" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6561" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6562">
+      <c r="A6562" s="6" t="n">
+        <v>44866.302083333336</v>
+      </c>
+      <c r="B6562" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6562" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6563">
+      <c r="A6563" s="6" t="n">
+        <v>44866.3125</v>
+      </c>
+      <c r="B6563" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6563" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6564">
+      <c r="A6564" s="6" t="n">
+        <v>44866.322916666664</v>
+      </c>
+      <c r="B6564" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6564" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6565">
+      <c r="A6565" s="6" t="n">
+        <v>44866.333333333336</v>
+      </c>
+      <c r="B6565" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6565" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6566">
+      <c r="A6566" s="6" t="n">
+        <v>44866.34375</v>
+      </c>
+      <c r="B6566" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6566" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="6567">
+      <c r="A6567" s="6" t="n">
+        <v>44866.354166666664</v>
+      </c>
+      <c r="B6567" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6567" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6568">
+      <c r="A6568" s="6" t="n">
+        <v>44866.364583333336</v>
+      </c>
+      <c r="B6568" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C6568" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6569">
+      <c r="A6569" s="6" t="n">
+        <v>44866.375</v>
+      </c>
+      <c r="B6569" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6569" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="6570">
+      <c r="A6570" s="6" t="n">
+        <v>44866.385416666664</v>
+      </c>
+      <c r="B6570" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6570" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6571">
+      <c r="A6571" s="6" t="n">
+        <v>44866.395833333336</v>
+      </c>
+      <c r="B6571" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6571" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="6572">
+      <c r="A6572" s="6" t="n">
+        <v>44866.40625</v>
+      </c>
+      <c r="B6572" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6572" s="1" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="6573">
+      <c r="A6573" s="6" t="n">
+        <v>44866.416666666664</v>
+      </c>
+      <c r="B6573" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6573" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6574">
+      <c r="A6574" s="6" t="n">
+        <v>44866.427083333336</v>
+      </c>
+      <c r="B6574" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6574" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6575">
+      <c r="A6575" s="6" t="n">
+        <v>44866.4375</v>
+      </c>
+      <c r="B6575" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6575" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6576">
+      <c r="A6576" s="6" t="n">
+        <v>44866.447916666664</v>
+      </c>
+      <c r="B6576" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6576" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6577">
+      <c r="A6577" s="6" t="n">
+        <v>44866.458333333336</v>
+      </c>
+      <c r="B6577" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6577" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6578">
+      <c r="A6578" s="6" t="n">
+        <v>44866.46875</v>
+      </c>
+      <c r="B6578" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6578" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6579">
+      <c r="A6579" s="6" t="n">
+        <v>44866.479166666664</v>
+      </c>
+      <c r="B6579" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6579" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6580">
+      <c r="A6580" s="6" t="n">
+        <v>44866.489583333336</v>
+      </c>
+      <c r="B6580" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6580" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6581">
+      <c r="A6581" s="6" t="n">
+        <v>44866.5</v>
+      </c>
+      <c r="B6581" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6581" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6582">
+      <c r="A6582" s="6" t="n">
+        <v>44866.510416666664</v>
+      </c>
+      <c r="B6582" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6582" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6583">
+      <c r="A6583" s="6" t="n">
+        <v>44866.520833333336</v>
+      </c>
+      <c r="B6583" s="1" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C6583" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6584">
+      <c r="A6584" s="6" t="n">
+        <v>44866.53125</v>
+      </c>
+      <c r="B6584" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6584" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6585">
+      <c r="A6585" s="6" t="n">
+        <v>44866.541666666664</v>
+      </c>
+      <c r="B6585" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6585" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6586">
+      <c r="A6586" s="6" t="n">
+        <v>44866.552083333336</v>
+      </c>
+      <c r="B6586" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6586" s="1" t="n">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="6587">
+      <c r="A6587" s="6" t="n">
+        <v>44866.5625</v>
+      </c>
+      <c r="B6587" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6587" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6588">
+      <c r="A6588" s="6" t="n">
+        <v>44866.572916666664</v>
+      </c>
+      <c r="B6588" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6588" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6589">
+      <c r="A6589" s="6" t="n">
+        <v>44866.583333333336</v>
+      </c>
+      <c r="B6589" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6589" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6590">
+      <c r="A6590" s="6" t="n">
+        <v>44866.59375</v>
+      </c>
+      <c r="B6590" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6590" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6591">
+      <c r="A6591" s="6" t="n">
+        <v>44866.604166666664</v>
+      </c>
+      <c r="B6591" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6591" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6592">
+      <c r="A6592" s="6" t="n">
+        <v>44866.614583333336</v>
+      </c>
+      <c r="B6592" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6592" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6593">
+      <c r="A6593" s="6" t="n">
+        <v>44866.625</v>
+      </c>
+      <c r="B6593" s="1" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C6593" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6594">
+      <c r="A6594" s="6" t="n">
+        <v>44866.635416666664</v>
+      </c>
+      <c r="B6594" s="1" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C6594" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6595">
+      <c r="A6595" s="6" t="n">
+        <v>44866.645833333336</v>
+      </c>
+      <c r="B6595" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C6595" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6596">
+      <c r="A6596" s="6" t="n">
+        <v>44866.65625</v>
+      </c>
+      <c r="B6596" s="1" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="C6596" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6597">
+      <c r="A6597" s="6" t="n">
+        <v>44866.666666666664</v>
+      </c>
+      <c r="B6597" s="1" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="C6597" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6598">
+      <c r="A6598" s="6" t="n">
+        <v>44866.677083333336</v>
+      </c>
+      <c r="B6598" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C6598" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6599">
+      <c r="A6599" s="6" t="n">
+        <v>44866.6875</v>
+      </c>
+      <c r="B6599" s="1" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C6599" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="6600">
+      <c r="A6600" s="6" t="n">
+        <v>44866.697916666664</v>
+      </c>
+      <c r="B6600" s="1" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="C6600" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6601">
+      <c r="A6601" s="6" t="n">
+        <v>44866.708333333336</v>
+      </c>
+      <c r="B6601" s="1" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="C6601" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6602">
+      <c r="A6602" s="6" t="n">
+        <v>44866.71875</v>
+      </c>
+      <c r="B6602" s="1" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="C6602" s="1" t="n">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="6603">
+      <c r="A6603" s="6" t="n">
+        <v>44866.729166666664</v>
+      </c>
+      <c r="B6603" s="1" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="C6603" s="1" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="6604">
+      <c r="A6604" s="6" t="n">
+        <v>44866.739583333336</v>
+      </c>
+      <c r="B6604" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6604" s="1" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="6605">
+      <c r="A6605" s="6" t="n">
+        <v>44866.75</v>
+      </c>
+      <c r="B6605" s="1" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="C6605" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6606">
+      <c r="A6606" s="6" t="n">
+        <v>44866.760416666664</v>
+      </c>
+      <c r="B6606" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6606" s="1" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="6607">
+      <c r="A6607" s="6" t="n">
+        <v>44866.770833333336</v>
+      </c>
+      <c r="B6607" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6607" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6608">
+      <c r="A6608" s="6" t="n">
+        <v>44866.78125</v>
+      </c>
+      <c r="B6608" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C6608" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6609">
+      <c r="A6609" s="6" t="n">
+        <v>44866.791666666664</v>
+      </c>
+      <c r="B6609" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6609" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6610">
+      <c r="A6610" s="6" t="n">
+        <v>44866.802083333336</v>
+      </c>
+      <c r="B6610" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6610" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6611">
+      <c r="A6611" s="6" t="n">
+        <v>44866.8125</v>
+      </c>
+      <c r="B6611" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6611" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6612">
+      <c r="A6612" s="6" t="n">
+        <v>44866.822916666664</v>
+      </c>
+      <c r="B6612" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6612" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6613">
+      <c r="A6613" s="6" t="n">
+        <v>44866.833333333336</v>
+      </c>
+      <c r="B6613" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6613" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6614">
+      <c r="A6614" s="6" t="n">
+        <v>44866.84375</v>
+      </c>
+      <c r="B6614" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6614" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6615">
+      <c r="A6615" s="6" t="n">
+        <v>44866.854166666664</v>
+      </c>
+      <c r="B6615" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6615" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6616">
+      <c r="A6616" s="6" t="n">
+        <v>44866.864583333336</v>
+      </c>
+      <c r="B6616" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6616" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6617">
+      <c r="A6617" s="6" t="n">
+        <v>44866.875</v>
+      </c>
+      <c r="B6617" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6617" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6618">
+      <c r="A6618" s="6" t="n">
+        <v>44866.885416666664</v>
+      </c>
+      <c r="B6618" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6618" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6619">
+      <c r="A6619" s="6" t="n">
+        <v>44866.895833333336</v>
+      </c>
+      <c r="B6619" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6619" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6620">
+      <c r="A6620" s="6" t="n">
+        <v>44866.90625</v>
+      </c>
+      <c r="B6620" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6620" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6621">
+      <c r="A6621" s="6" t="n">
+        <v>44866.916666666664</v>
+      </c>
+      <c r="B6621" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6621" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6622">
+      <c r="A6622" s="6" t="n">
+        <v>44866.927083333336</v>
+      </c>
+      <c r="B6622" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6622" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6623">
+      <c r="A6623" s="6" t="n">
+        <v>44866.9375</v>
+      </c>
+      <c r="B6623" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6623" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6624">
+      <c r="A6624" s="6" t="n">
+        <v>44866.947916666664</v>
+      </c>
+      <c r="B6624" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6624" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6625">
+      <c r="A6625" s="6" t="n">
+        <v>44866.958333333336</v>
+      </c>
+      <c r="B6625" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6625" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6626">
+      <c r="A6626" s="6" t="n">
+        <v>44866.96875</v>
+      </c>
+      <c r="B6626" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6626" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6627">
+      <c r="A6627" s="6" t="n">
+        <v>44866.979166666664</v>
+      </c>
+      <c r="B6627" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6627" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6628">
+      <c r="A6628" s="6" t="n">
+        <v>44866.989583333336</v>
+      </c>
+      <c r="B6628" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6628" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6629">
+      <c r="A6629" s="6" t="n">
+        <v>44867.0</v>
+      </c>
+      <c r="B6629" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6629" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6630">
+      <c r="A6630" s="6" t="n">
+        <v>44867.010416666664</v>
+      </c>
+      <c r="B6630" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6630" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6631">
+      <c r="A6631" s="6" t="n">
+        <v>44867.020833333336</v>
+      </c>
+      <c r="B6631" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6631" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6632">
+      <c r="A6632" s="6" t="n">
+        <v>44867.03125</v>
+      </c>
+      <c r="B6632" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6632" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6633">
+      <c r="A6633" s="6" t="n">
+        <v>44867.041666666664</v>
+      </c>
+      <c r="B6633" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6633" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6634">
+      <c r="A6634" s="6" t="n">
+        <v>44867.052083333336</v>
+      </c>
+      <c r="B6634" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6634" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6635">
+      <c r="A6635" s="6" t="n">
+        <v>44867.0625</v>
+      </c>
+      <c r="B6635" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6635" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6636">
+      <c r="A6636" s="6" t="n">
+        <v>44867.072916666664</v>
+      </c>
+      <c r="B6636" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6636" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6637">
+      <c r="A6637" s="6" t="n">
+        <v>44867.083333333336</v>
+      </c>
+      <c r="B6637" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6637" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6638">
+      <c r="A6638" s="6" t="n">
+        <v>44867.09375</v>
+      </c>
+      <c r="B6638" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6638" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6639">
+      <c r="A6639" s="6" t="n">
+        <v>44867.104166666664</v>
+      </c>
+      <c r="B6639" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6639" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6640">
+      <c r="A6640" s="6" t="n">
+        <v>44867.114583333336</v>
+      </c>
+      <c r="B6640" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6640" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6641">
+      <c r="A6641" s="6" t="n">
+        <v>44867.125</v>
+      </c>
+      <c r="B6641" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6641" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6642">
+      <c r="A6642" s="6" t="n">
+        <v>44867.135416666664</v>
+      </c>
+      <c r="B6642" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6642" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6643">
+      <c r="A6643" s="6" t="n">
+        <v>44867.145833333336</v>
+      </c>
+      <c r="B6643" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6643" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6644">
+      <c r="A6644" s="6" t="n">
+        <v>44867.15625</v>
+      </c>
+      <c r="B6644" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6644" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6645">
+      <c r="A6645" s="6" t="n">
+        <v>44867.166666666664</v>
+      </c>
+      <c r="B6645" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6645" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6646">
+      <c r="A6646" s="6" t="n">
+        <v>44867.177083333336</v>
+      </c>
+      <c r="B6646" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6646" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6647">
+      <c r="A6647" s="6" t="n">
+        <v>44867.1875</v>
+      </c>
+      <c r="B6647" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6647" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6648">
+      <c r="A6648" s="6" t="n">
+        <v>44867.197916666664</v>
+      </c>
+      <c r="B6648" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6648" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6649">
+      <c r="A6649" s="6" t="n">
+        <v>44867.208333333336</v>
+      </c>
+      <c r="B6649" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6649" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6650">
+      <c r="A6650" s="6" t="n">
+        <v>44867.21875</v>
+      </c>
+      <c r="B6650" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6650" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6651">
+      <c r="A6651" s="6" t="n">
+        <v>44867.229166666664</v>
+      </c>
+      <c r="B6651" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6651" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6652">
+      <c r="A6652" s="6" t="n">
+        <v>44867.239583333336</v>
+      </c>
+      <c r="B6652" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6652" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6653">
+      <c r="A6653" s="6" t="n">
+        <v>44867.25</v>
+      </c>
+      <c r="B6653" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6653" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6654">
+      <c r="A6654" s="6" t="n">
+        <v>44867.260416666664</v>
+      </c>
+      <c r="B6654" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6654" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6655">
+      <c r="A6655" s="6" t="n">
+        <v>44867.270833333336</v>
+      </c>
+      <c r="B6655" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6655" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6656">
+      <c r="A6656" s="6" t="n">
+        <v>44867.28125</v>
+      </c>
+      <c r="B6656" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6656" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6657">
+      <c r="A6657" s="6" t="n">
+        <v>44867.291666666664</v>
+      </c>
+      <c r="B6657" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6657" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6658">
+      <c r="A6658" s="6" t="n">
+        <v>44867.302083333336</v>
+      </c>
+      <c r="B6658" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6658" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6659">
+      <c r="A6659" s="6" t="n">
+        <v>44867.3125</v>
+      </c>
+      <c r="B6659" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6659" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6660">
+      <c r="A6660" s="6" t="n">
+        <v>44867.322916666664</v>
+      </c>
+      <c r="B6660" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6660" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6661">
+      <c r="A6661" s="6" t="n">
+        <v>44867.333333333336</v>
+      </c>
+      <c r="B6661" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C6661" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6662">
+      <c r="A6662" s="6" t="n">
+        <v>44867.34375</v>
+      </c>
+      <c r="B6662" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6662" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6663">
+      <c r="A6663" s="6" t="n">
+        <v>44867.354166666664</v>
+      </c>
+      <c r="B6663" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6663" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6664">
+      <c r="A6664" s="6" t="n">
+        <v>44867.364583333336</v>
+      </c>
+      <c r="B6664" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6664" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="6665">
+      <c r="A6665" s="6" t="n">
+        <v>44867.375</v>
+      </c>
+      <c r="B6665" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C6665" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6666">
+      <c r="A6666" s="6" t="n">
+        <v>44867.385416666664</v>
+      </c>
+      <c r="B6666" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6666" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6667">
+      <c r="A6667" s="6" t="n">
+        <v>44867.395833333336</v>
+      </c>
+      <c r="B6667" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6667" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6668">
+      <c r="A6668" s="6" t="n">
+        <v>44867.40625</v>
+      </c>
+      <c r="B6668" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6668" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="6669">
+      <c r="A6669" s="6" t="n">
+        <v>44867.416666666664</v>
+      </c>
+      <c r="B6669" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6669" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="6670">
+      <c r="A6670" s="6" t="n">
+        <v>44867.427083333336</v>
+      </c>
+      <c r="B6670" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6670" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6671">
+      <c r="A6671" s="6" t="n">
+        <v>44867.4375</v>
+      </c>
+      <c r="B6671" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6671" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6672">
+      <c r="A6672" s="6" t="n">
+        <v>44867.447916666664</v>
+      </c>
+      <c r="B6672" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6672" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6673">
+      <c r="A6673" s="6" t="n">
+        <v>44867.458333333336</v>
+      </c>
+      <c r="B6673" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6673" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6674">
+      <c r="A6674" s="6" t="n">
+        <v>44867.46875</v>
+      </c>
+      <c r="B6674" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6674" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6675">
+      <c r="A6675" s="6" t="n">
+        <v>44867.479166666664</v>
+      </c>
+      <c r="B6675" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C6675" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6676">
+      <c r="A6676" s="6" t="n">
+        <v>44867.489583333336</v>
+      </c>
+      <c r="B6676" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6676" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6677">
+      <c r="A6677" s="6" t="n">
+        <v>44867.5</v>
+      </c>
+      <c r="B6677" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6677" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6678">
+      <c r="A6678" s="6" t="n">
+        <v>44867.510416666664</v>
+      </c>
+      <c r="B6678" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6678" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6679">
+      <c r="A6679" s="6" t="n">
+        <v>44867.520833333336</v>
+      </c>
+      <c r="B6679" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6679" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="6680">
+      <c r="A6680" s="6" t="n">
+        <v>44867.53125</v>
+      </c>
+      <c r="B6680" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6680" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6681">
+      <c r="A6681" s="6" t="n">
+        <v>44867.541666666664</v>
+      </c>
+      <c r="B6681" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6681" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6682">
+      <c r="A6682" s="6" t="n">
+        <v>44867.552083333336</v>
+      </c>
+      <c r="B6682" s="1"/>
+      <c r="C6682" s="1"/>
+    </row>
+    <row r="6683">
+      <c r="A6683" s="6" t="n">
+        <v>44867.5625</v>
+      </c>
+      <c r="B6683" s="1"/>
+      <c r="C6683" s="1"/>
+    </row>
+    <row r="6684">
+      <c r="A6684" s="6" t="n">
+        <v>44867.572916666664</v>
+      </c>
+      <c r="B6684" s="1"/>
+      <c r="C6684" s="1"/>
+    </row>
+    <row r="6685">
+      <c r="A6685" s="6" t="n">
+        <v>44867.583333333336</v>
+      </c>
+      <c r="B6685" s="1"/>
+      <c r="C6685" s="1"/>
+    </row>
+    <row r="6686">
+      <c r="A6686" s="6" t="n">
+        <v>44867.59375</v>
+      </c>
+      <c r="B6686" s="1"/>
+      <c r="C6686" s="1"/>
+    </row>
+    <row r="6687">
+      <c r="A6687" s="6" t="n">
+        <v>44867.604166666664</v>
+      </c>
+      <c r="B6687" s="1"/>
+      <c r="C6687" s="1"/>
+    </row>
+    <row r="6688">
+      <c r="A6688" s="6" t="n">
+        <v>44867.614583333336</v>
+      </c>
+      <c r="B6688" s="1"/>
+      <c r="C6688" s="1"/>
+    </row>
+    <row r="6689">
+      <c r="A6689" s="6" t="n">
+        <v>44867.625</v>
+      </c>
+      <c r="B6689" s="1"/>
+      <c r="C6689" s="1"/>
+    </row>
+    <row r="6690">
+      <c r="A6690" s="6" t="n">
+        <v>44867.635416666664</v>
+      </c>
+      <c r="B6690" s="1"/>
+      <c r="C6690" s="1"/>
+    </row>
+    <row r="6691">
+      <c r="A6691" s="6" t="n">
+        <v>44867.645833333336</v>
+      </c>
+      <c r="B6691" s="1"/>
+      <c r="C6691" s="1"/>
+    </row>
+    <row r="6692">
+      <c r="A6692" s="6" t="n">
+        <v>44867.65625</v>
+      </c>
+      <c r="B6692" s="1"/>
+      <c r="C6692" s="1"/>
+    </row>
+    <row r="6693">
+      <c r="A6693" s="6" t="n">
+        <v>44867.666666666664</v>
+      </c>
+      <c r="B6693" s="1"/>
+      <c r="C6693" s="1"/>
+    </row>
+    <row r="6694">
+      <c r="A6694" s="6" t="n">
+        <v>44867.677083333336</v>
+      </c>
+      <c r="B6694" s="1"/>
+      <c r="C6694" s="1"/>
+    </row>
+    <row r="6695">
+      <c r="A6695" s="6" t="n">
+        <v>44867.6875</v>
+      </c>
+      <c r="B6695" s="1"/>
+      <c r="C6695" s="1"/>
+    </row>
+    <row r="6696">
+      <c r="A6696" s="6" t="n">
+        <v>44867.697916666664</v>
+      </c>
+      <c r="B6696" s="1"/>
+      <c r="C6696" s="1"/>
+    </row>
+    <row r="6697">
+      <c r="A6697" s="6" t="n">
+        <v>44867.708333333336</v>
+      </c>
+      <c r="B6697" s="1"/>
+      <c r="C6697" s="1"/>
+    </row>
+    <row r="6698">
+      <c r="A6698" s="6" t="n">
+        <v>44867.71875</v>
+      </c>
+      <c r="B6698" s="1"/>
+      <c r="C6698" s="1"/>
+    </row>
+    <row r="6699">
+      <c r="A6699" s="6" t="n">
+        <v>44867.729166666664</v>
+      </c>
+      <c r="B6699" s="1"/>
+      <c r="C6699" s="1"/>
+    </row>
+    <row r="6700">
+      <c r="A6700" s="6" t="n">
+        <v>44867.739583333336</v>
+      </c>
+      <c r="B6700" s="1"/>
+      <c r="C6700" s="1"/>
+    </row>
+    <row r="6701">
+      <c r="A6701" s="6" t="n">
+        <v>44867.75</v>
+      </c>
+      <c r="B6701" s="1"/>
+      <c r="C6701" s="1"/>
+    </row>
+    <row r="6702">
+      <c r="A6702" s="6" t="n">
+        <v>44867.760416666664</v>
+      </c>
+      <c r="B6702" s="1"/>
+      <c r="C6702" s="1"/>
+    </row>
+    <row r="6703">
+      <c r="A6703" s="6" t="n">
+        <v>44867.770833333336</v>
+      </c>
+      <c r="B6703" s="1"/>
+      <c r="C6703" s="1"/>
+    </row>
+    <row r="6704">
+      <c r="A6704" s="6" t="n">
+        <v>44867.78125</v>
+      </c>
+      <c r="B6704" s="1"/>
+      <c r="C6704" s="1"/>
+    </row>
+    <row r="6705">
+      <c r="A6705" s="6" t="n">
+        <v>44867.791666666664</v>
+      </c>
+      <c r="B6705" s="1"/>
+      <c r="C6705" s="1"/>
+    </row>
+    <row r="6706">
+      <c r="A6706" s="6" t="n">
+        <v>44867.802083333336</v>
+      </c>
+      <c r="B6706" s="1"/>
+      <c r="C6706" s="1"/>
+    </row>
+    <row r="6707">
+      <c r="A6707" s="6" t="n">
+        <v>44867.8125</v>
+      </c>
+      <c r="B6707" s="1"/>
+      <c r="C6707" s="1"/>
+    </row>
+    <row r="6708">
+      <c r="A6708" s="6" t="n">
+        <v>44867.822916666664</v>
+      </c>
+      <c r="B6708" s="1"/>
+      <c r="C6708" s="1"/>
+    </row>
+    <row r="6709">
+      <c r="A6709" s="6" t="n">
+        <v>44867.833333333336</v>
+      </c>
+      <c r="B6709" s="1"/>
+      <c r="C6709" s="1"/>
+    </row>
+    <row r="6710">
+      <c r="A6710" s="6" t="n">
+        <v>44867.84375</v>
+      </c>
+      <c r="B6710" s="1"/>
+      <c r="C6710" s="1"/>
+    </row>
+    <row r="6711">
+      <c r="A6711" s="6" t="n">
+        <v>44867.854166666664</v>
+      </c>
+      <c r="B6711" s="1"/>
+      <c r="C6711" s="1"/>
+    </row>
+    <row r="6712">
+      <c r="A6712" s="6" t="n">
+        <v>44867.864583333336</v>
+      </c>
+      <c r="B6712" s="1"/>
+      <c r="C6712" s="1"/>
+    </row>
+    <row r="6713">
+      <c r="A6713" s="6" t="n">
+        <v>44867.875</v>
+      </c>
+      <c r="B6713" s="1"/>
+      <c r="C6713" s="1"/>
+    </row>
+    <row r="6714">
+      <c r="A6714" s="6" t="n">
+        <v>44867.885416666664</v>
+      </c>
+      <c r="B6714" s="1"/>
+      <c r="C6714" s="1"/>
+    </row>
+    <row r="6715">
+      <c r="A6715" s="6" t="n">
+        <v>44867.895833333336</v>
+      </c>
+      <c r="B6715" s="1"/>
+      <c r="C6715" s="1"/>
+    </row>
+    <row r="6716">
+      <c r="A6716" s="6" t="n">
+        <v>44867.90625</v>
+      </c>
+      <c r="B6716" s="1"/>
+      <c r="C6716" s="1"/>
+    </row>
+    <row r="6717">
+      <c r="A6717" s="6" t="n">
+        <v>44867.916666666664</v>
+      </c>
+      <c r="B6717" s="1"/>
+      <c r="C6717" s="1"/>
+    </row>
+    <row r="6718">
+      <c r="A6718" s="6" t="n">
+        <v>44867.927083333336</v>
+      </c>
+      <c r="B6718" s="1"/>
+      <c r="C6718" s="1"/>
+    </row>
+    <row r="6719">
+      <c r="A6719" s="6" t="n">
+        <v>44867.9375</v>
+      </c>
+      <c r="B6719" s="1"/>
+      <c r="C6719" s="1"/>
+    </row>
+    <row r="6720">
+      <c r="A6720" s="6" t="n">
+        <v>44867.947916666664</v>
+      </c>
+      <c r="B6720" s="1"/>
+      <c r="C6720" s="1"/>
+    </row>
+    <row r="6721">
+      <c r="A6721" s="6" t="n">
+        <v>44867.958333333336</v>
+      </c>
+      <c r="B6721" s="1"/>
+      <c r="C6721" s="1"/>
+    </row>
+    <row r="6722">
+      <c r="A6722" s="6" t="n">
+        <v>44867.96875</v>
+      </c>
+      <c r="B6722" s="1"/>
+      <c r="C6722" s="1"/>
+    </row>
+    <row r="6723">
+      <c r="A6723" s="6" t="n">
+        <v>44867.979166666664</v>
+      </c>
+      <c r="B6723" s="1"/>
+      <c r="C6723" s="1"/>
+    </row>
+    <row r="6724">
+      <c r="A6724" s="6" t="n">
+        <v>44867.989583333336</v>
+      </c>
+      <c r="B6724" s="1"/>
+      <c r="C6724" s="1"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
Update Ann Arbor data.
</commit_message>
<xml_diff>
--- a/data/counter/export_data_domain_7992.xlsx
+++ b/data/counter/export_data_domain_7992.xlsx
@@ -88340,344 +88340,4764 @@
       <c r="A8020" s="6" t="n">
         <v>44881.489583333336</v>
       </c>
-      <c r="B8020" s="1"/>
-      <c r="C8020" s="1"/>
+      <c r="B8020" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8020" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="8021">
       <c r="A8021" s="6" t="n">
         <v>44881.5</v>
       </c>
-      <c r="B8021" s="1"/>
-      <c r="C8021" s="1"/>
+      <c r="B8021" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8021" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="8022">
       <c r="A8022" s="6" t="n">
         <v>44881.510416666664</v>
       </c>
-      <c r="B8022" s="1"/>
-      <c r="C8022" s="1"/>
+      <c r="B8022" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8022" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="8023">
       <c r="A8023" s="6" t="n">
         <v>44881.520833333336</v>
       </c>
-      <c r="B8023" s="1"/>
-      <c r="C8023" s="1"/>
+      <c r="B8023" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8023" s="1" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="8024">
       <c r="A8024" s="6" t="n">
         <v>44881.53125</v>
       </c>
-      <c r="B8024" s="1"/>
-      <c r="C8024" s="1"/>
+      <c r="B8024" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8024" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="8025">
       <c r="A8025" s="6" t="n">
         <v>44881.541666666664</v>
       </c>
-      <c r="B8025" s="1"/>
-      <c r="C8025" s="1"/>
+      <c r="B8025" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C8025" s="1" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="8026">
       <c r="A8026" s="6" t="n">
         <v>44881.552083333336</v>
       </c>
-      <c r="B8026" s="1"/>
-      <c r="C8026" s="1"/>
+      <c r="B8026" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8026" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="8027">
       <c r="A8027" s="6" t="n">
         <v>44881.5625</v>
       </c>
-      <c r="B8027" s="1"/>
-      <c r="C8027" s="1"/>
+      <c r="B8027" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8027" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="8028">
       <c r="A8028" s="6" t="n">
         <v>44881.572916666664</v>
       </c>
-      <c r="B8028" s="1"/>
-      <c r="C8028" s="1"/>
+      <c r="B8028" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8028" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="8029">
       <c r="A8029" s="6" t="n">
         <v>44881.583333333336</v>
       </c>
-      <c r="B8029" s="1"/>
-      <c r="C8029" s="1"/>
+      <c r="B8029" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C8029" s="1" t="n">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="8030">
       <c r="A8030" s="6" t="n">
         <v>44881.59375</v>
       </c>
-      <c r="B8030" s="1"/>
-      <c r="C8030" s="1"/>
+      <c r="B8030" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8030" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="8031">
       <c r="A8031" s="6" t="n">
         <v>44881.604166666664</v>
       </c>
-      <c r="B8031" s="1"/>
-      <c r="C8031" s="1"/>
+      <c r="B8031" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8031" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="8032">
       <c r="A8032" s="6" t="n">
         <v>44881.614583333336</v>
       </c>
-      <c r="B8032" s="1"/>
-      <c r="C8032" s="1"/>
+      <c r="B8032" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C8032" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="8033">
       <c r="A8033" s="6" t="n">
         <v>44881.625</v>
       </c>
-      <c r="B8033" s="1"/>
-      <c r="C8033" s="1"/>
+      <c r="B8033" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C8033" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="8034">
       <c r="A8034" s="6" t="n">
         <v>44881.635416666664</v>
       </c>
-      <c r="B8034" s="1"/>
-      <c r="C8034" s="1"/>
+      <c r="B8034" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8034" s="1" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="8035">
       <c r="A8035" s="6" t="n">
         <v>44881.645833333336</v>
       </c>
-      <c r="B8035" s="1"/>
-      <c r="C8035" s="1"/>
+      <c r="B8035" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C8035" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="8036">
       <c r="A8036" s="6" t="n">
         <v>44881.65625</v>
       </c>
-      <c r="B8036" s="1"/>
-      <c r="C8036" s="1"/>
+      <c r="B8036" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8036" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="8037">
       <c r="A8037" s="6" t="n">
         <v>44881.666666666664</v>
       </c>
-      <c r="B8037" s="1"/>
-      <c r="C8037" s="1"/>
+      <c r="B8037" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C8037" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="8038">
       <c r="A8038" s="6" t="n">
         <v>44881.677083333336</v>
       </c>
-      <c r="B8038" s="1"/>
-      <c r="C8038" s="1"/>
+      <c r="B8038" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C8038" s="1" t="n">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="8039">
       <c r="A8039" s="6" t="n">
         <v>44881.6875</v>
       </c>
-      <c r="B8039" s="1"/>
-      <c r="C8039" s="1"/>
+      <c r="B8039" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C8039" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="8040">
       <c r="A8040" s="6" t="n">
         <v>44881.697916666664</v>
       </c>
-      <c r="B8040" s="1"/>
-      <c r="C8040" s="1"/>
+      <c r="B8040" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C8040" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="8041">
       <c r="A8041" s="6" t="n">
         <v>44881.708333333336</v>
       </c>
-      <c r="B8041" s="1"/>
-      <c r="C8041" s="1"/>
+      <c r="B8041" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C8041" s="1" t="n">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="8042">
       <c r="A8042" s="6" t="n">
         <v>44881.71875</v>
       </c>
-      <c r="B8042" s="1"/>
-      <c r="C8042" s="1"/>
+      <c r="B8042" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C8042" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="8043">
       <c r="A8043" s="6" t="n">
         <v>44881.729166666664</v>
       </c>
-      <c r="B8043" s="1"/>
-      <c r="C8043" s="1"/>
+      <c r="B8043" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C8043" s="1" t="n">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="8044">
       <c r="A8044" s="6" t="n">
         <v>44881.739583333336</v>
       </c>
-      <c r="B8044" s="1"/>
-      <c r="C8044" s="1"/>
+      <c r="B8044" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C8044" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="8045">
       <c r="A8045" s="6" t="n">
         <v>44881.75</v>
       </c>
-      <c r="B8045" s="1"/>
-      <c r="C8045" s="1"/>
+      <c r="B8045" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8045" s="1" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="8046">
       <c r="A8046" s="6" t="n">
         <v>44881.760416666664</v>
       </c>
-      <c r="B8046" s="1"/>
-      <c r="C8046" s="1"/>
+      <c r="B8046" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C8046" s="1" t="n">
+        <v>4.0</v>
+      </c>
     </row>
     <row r="8047">
       <c r="A8047" s="6" t="n">
         <v>44881.770833333336</v>
       </c>
-      <c r="B8047" s="1"/>
-      <c r="C8047" s="1"/>
+      <c r="B8047" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C8047" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="8048">
       <c r="A8048" s="6" t="n">
         <v>44881.78125</v>
       </c>
-      <c r="B8048" s="1"/>
-      <c r="C8048" s="1"/>
+      <c r="B8048" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8048" s="1" t="n">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="8049">
       <c r="A8049" s="6" t="n">
         <v>44881.791666666664</v>
       </c>
-      <c r="B8049" s="1"/>
-      <c r="C8049" s="1"/>
+      <c r="B8049" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C8049" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="8050">
       <c r="A8050" s="6" t="n">
         <v>44881.802083333336</v>
       </c>
-      <c r="B8050" s="1"/>
-      <c r="C8050" s="1"/>
+      <c r="B8050" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8050" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="8051">
       <c r="A8051" s="6" t="n">
         <v>44881.8125</v>
       </c>
-      <c r="B8051" s="1"/>
-      <c r="C8051" s="1"/>
+      <c r="B8051" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C8051" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="8052">
       <c r="A8052" s="6" t="n">
         <v>44881.822916666664</v>
       </c>
-      <c r="B8052" s="1"/>
-      <c r="C8052" s="1"/>
+      <c r="B8052" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8052" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="8053">
       <c r="A8053" s="6" t="n">
         <v>44881.833333333336</v>
       </c>
-      <c r="B8053" s="1"/>
-      <c r="C8053" s="1"/>
+      <c r="B8053" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8053" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="8054">
       <c r="A8054" s="6" t="n">
         <v>44881.84375</v>
       </c>
-      <c r="B8054" s="1"/>
-      <c r="C8054" s="1"/>
+      <c r="B8054" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8054" s="1" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="8055">
       <c r="A8055" s="6" t="n">
         <v>44881.854166666664</v>
       </c>
-      <c r="B8055" s="1"/>
-      <c r="C8055" s="1"/>
+      <c r="B8055" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8055" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="8056">
       <c r="A8056" s="6" t="n">
         <v>44881.864583333336</v>
       </c>
-      <c r="B8056" s="1"/>
-      <c r="C8056" s="1"/>
+      <c r="B8056" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C8056" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="8057">
       <c r="A8057" s="6" t="n">
         <v>44881.875</v>
       </c>
-      <c r="B8057" s="1"/>
-      <c r="C8057" s="1"/>
+      <c r="B8057" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C8057" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="8058">
       <c r="A8058" s="6" t="n">
         <v>44881.885416666664</v>
       </c>
-      <c r="B8058" s="1"/>
-      <c r="C8058" s="1"/>
+      <c r="B8058" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C8058" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="8059">
       <c r="A8059" s="6" t="n">
         <v>44881.895833333336</v>
       </c>
-      <c r="B8059" s="1"/>
-      <c r="C8059" s="1"/>
+      <c r="B8059" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8059" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="8060">
       <c r="A8060" s="6" t="n">
         <v>44881.90625</v>
       </c>
-      <c r="B8060" s="1"/>
-      <c r="C8060" s="1"/>
+      <c r="B8060" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8060" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="8061">
       <c r="A8061" s="6" t="n">
         <v>44881.916666666664</v>
       </c>
-      <c r="B8061" s="1"/>
-      <c r="C8061" s="1"/>
+      <c r="B8061" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8061" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="8062">
       <c r="A8062" s="6" t="n">
         <v>44881.927083333336</v>
       </c>
-      <c r="B8062" s="1"/>
-      <c r="C8062" s="1"/>
+      <c r="B8062" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8062" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="8063">
       <c r="A8063" s="6" t="n">
         <v>44881.9375</v>
       </c>
-      <c r="B8063" s="1"/>
-      <c r="C8063" s="1"/>
+      <c r="B8063" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8063" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="8064">
       <c r="A8064" s="6" t="n">
         <v>44881.947916666664</v>
       </c>
-      <c r="B8064" s="1"/>
-      <c r="C8064" s="1"/>
+      <c r="B8064" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8064" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="8065">
       <c r="A8065" s="6" t="n">
         <v>44881.958333333336</v>
       </c>
-      <c r="B8065" s="1"/>
-      <c r="C8065" s="1"/>
+      <c r="B8065" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8065" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="8066">
       <c r="A8066" s="6" t="n">
         <v>44881.96875</v>
       </c>
-      <c r="B8066" s="1"/>
-      <c r="C8066" s="1"/>
+      <c r="B8066" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8066" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="8067">
       <c r="A8067" s="6" t="n">
         <v>44881.979166666664</v>
       </c>
-      <c r="B8067" s="1"/>
-      <c r="C8067" s="1"/>
+      <c r="B8067" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8067" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="8068">
       <c r="A8068" s="6" t="n">
         <v>44881.989583333336</v>
       </c>
-      <c r="B8068" s="1"/>
-      <c r="C8068" s="1"/>
+      <c r="B8068" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8068" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8069">
+      <c r="A8069" s="6" t="n">
+        <v>44882.0</v>
+      </c>
+      <c r="B8069" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8069" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8070">
+      <c r="A8070" s="6" t="n">
+        <v>44882.010416666664</v>
+      </c>
+      <c r="B8070" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8070" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8071">
+      <c r="A8071" s="6" t="n">
+        <v>44882.020833333336</v>
+      </c>
+      <c r="B8071" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8071" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8072">
+      <c r="A8072" s="6" t="n">
+        <v>44882.03125</v>
+      </c>
+      <c r="B8072" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8072" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8073">
+      <c r="A8073" s="6" t="n">
+        <v>44882.041666666664</v>
+      </c>
+      <c r="B8073" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8073" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8074">
+      <c r="A8074" s="6" t="n">
+        <v>44882.052083333336</v>
+      </c>
+      <c r="B8074" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8074" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8075">
+      <c r="A8075" s="6" t="n">
+        <v>44882.0625</v>
+      </c>
+      <c r="B8075" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C8075" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8076">
+      <c r="A8076" s="6" t="n">
+        <v>44882.072916666664</v>
+      </c>
+      <c r="B8076" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8076" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8077">
+      <c r="A8077" s="6" t="n">
+        <v>44882.083333333336</v>
+      </c>
+      <c r="B8077" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8077" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8078">
+      <c r="A8078" s="6" t="n">
+        <v>44882.09375</v>
+      </c>
+      <c r="B8078" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8078" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8079">
+      <c r="A8079" s="6" t="n">
+        <v>44882.104166666664</v>
+      </c>
+      <c r="B8079" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8079" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8080">
+      <c r="A8080" s="6" t="n">
+        <v>44882.114583333336</v>
+      </c>
+      <c r="B8080" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8080" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8081">
+      <c r="A8081" s="6" t="n">
+        <v>44882.125</v>
+      </c>
+      <c r="B8081" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8081" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8082">
+      <c r="A8082" s="6" t="n">
+        <v>44882.135416666664</v>
+      </c>
+      <c r="B8082" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8082" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8083">
+      <c r="A8083" s="6" t="n">
+        <v>44882.145833333336</v>
+      </c>
+      <c r="B8083" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8083" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8084">
+      <c r="A8084" s="6" t="n">
+        <v>44882.15625</v>
+      </c>
+      <c r="B8084" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8084" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8085">
+      <c r="A8085" s="6" t="n">
+        <v>44882.166666666664</v>
+      </c>
+      <c r="B8085" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8085" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8086">
+      <c r="A8086" s="6" t="n">
+        <v>44882.177083333336</v>
+      </c>
+      <c r="B8086" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8086" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8087">
+      <c r="A8087" s="6" t="n">
+        <v>44882.1875</v>
+      </c>
+      <c r="B8087" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8087" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8088">
+      <c r="A8088" s="6" t="n">
+        <v>44882.197916666664</v>
+      </c>
+      <c r="B8088" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8088" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8089">
+      <c r="A8089" s="6" t="n">
+        <v>44882.208333333336</v>
+      </c>
+      <c r="B8089" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8089" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8090">
+      <c r="A8090" s="6" t="n">
+        <v>44882.21875</v>
+      </c>
+      <c r="B8090" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8090" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8091">
+      <c r="A8091" s="6" t="n">
+        <v>44882.229166666664</v>
+      </c>
+      <c r="B8091" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8091" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8092">
+      <c r="A8092" s="6" t="n">
+        <v>44882.239583333336</v>
+      </c>
+      <c r="B8092" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8092" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8093">
+      <c r="A8093" s="6" t="n">
+        <v>44882.25</v>
+      </c>
+      <c r="B8093" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8093" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8094">
+      <c r="A8094" s="6" t="n">
+        <v>44882.260416666664</v>
+      </c>
+      <c r="B8094" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8094" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8095">
+      <c r="A8095" s="6" t="n">
+        <v>44882.270833333336</v>
+      </c>
+      <c r="B8095" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8095" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8096">
+      <c r="A8096" s="6" t="n">
+        <v>44882.28125</v>
+      </c>
+      <c r="B8096" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8096" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8097">
+      <c r="A8097" s="6" t="n">
+        <v>44882.291666666664</v>
+      </c>
+      <c r="B8097" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8097" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8098">
+      <c r="A8098" s="6" t="n">
+        <v>44882.302083333336</v>
+      </c>
+      <c r="B8098" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8098" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="8099">
+      <c r="A8099" s="6" t="n">
+        <v>44882.3125</v>
+      </c>
+      <c r="B8099" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8099" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8100">
+      <c r="A8100" s="6" t="n">
+        <v>44882.322916666664</v>
+      </c>
+      <c r="B8100" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C8100" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8101">
+      <c r="A8101" s="6" t="n">
+        <v>44882.333333333336</v>
+      </c>
+      <c r="B8101" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C8101" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8102">
+      <c r="A8102" s="6" t="n">
+        <v>44882.34375</v>
+      </c>
+      <c r="B8102" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8102" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8103">
+      <c r="A8103" s="6" t="n">
+        <v>44882.354166666664</v>
+      </c>
+      <c r="B8103" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C8103" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8104">
+      <c r="A8104" s="6" t="n">
+        <v>44882.364583333336</v>
+      </c>
+      <c r="B8104" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8104" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8105">
+      <c r="A8105" s="6" t="n">
+        <v>44882.375</v>
+      </c>
+      <c r="B8105" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8105" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8106">
+      <c r="A8106" s="6" t="n">
+        <v>44882.385416666664</v>
+      </c>
+      <c r="B8106" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8106" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="8107">
+      <c r="A8107" s="6" t="n">
+        <v>44882.395833333336</v>
+      </c>
+      <c r="B8107" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8107" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8108">
+      <c r="A8108" s="6" t="n">
+        <v>44882.40625</v>
+      </c>
+      <c r="B8108" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8108" s="1" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="8109">
+      <c r="A8109" s="6" t="n">
+        <v>44882.416666666664</v>
+      </c>
+      <c r="B8109" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8109" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8110">
+      <c r="A8110" s="6" t="n">
+        <v>44882.427083333336</v>
+      </c>
+      <c r="B8110" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8110" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8111">
+      <c r="A8111" s="6" t="n">
+        <v>44882.4375</v>
+      </c>
+      <c r="B8111" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8111" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8112">
+      <c r="A8112" s="6" t="n">
+        <v>44882.447916666664</v>
+      </c>
+      <c r="B8112" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8112" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8113">
+      <c r="A8113" s="6" t="n">
+        <v>44882.458333333336</v>
+      </c>
+      <c r="B8113" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8113" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8114">
+      <c r="A8114" s="6" t="n">
+        <v>44882.46875</v>
+      </c>
+      <c r="B8114" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8114" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8115">
+      <c r="A8115" s="6" t="n">
+        <v>44882.479166666664</v>
+      </c>
+      <c r="B8115" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C8115" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8116">
+      <c r="A8116" s="6" t="n">
+        <v>44882.489583333336</v>
+      </c>
+      <c r="B8116" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8116" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8117">
+      <c r="A8117" s="6" t="n">
+        <v>44882.5</v>
+      </c>
+      <c r="B8117" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8117" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8118">
+      <c r="A8118" s="6" t="n">
+        <v>44882.510416666664</v>
+      </c>
+      <c r="B8118" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8118" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8119">
+      <c r="A8119" s="6" t="n">
+        <v>44882.520833333336</v>
+      </c>
+      <c r="B8119" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8119" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8120">
+      <c r="A8120" s="6" t="n">
+        <v>44882.53125</v>
+      </c>
+      <c r="B8120" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8120" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8121">
+      <c r="A8121" s="6" t="n">
+        <v>44882.541666666664</v>
+      </c>
+      <c r="B8121" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C8121" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8122">
+      <c r="A8122" s="6" t="n">
+        <v>44882.552083333336</v>
+      </c>
+      <c r="B8122" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8122" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8123">
+      <c r="A8123" s="6" t="n">
+        <v>44882.5625</v>
+      </c>
+      <c r="B8123" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8123" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8124">
+      <c r="A8124" s="6" t="n">
+        <v>44882.572916666664</v>
+      </c>
+      <c r="B8124" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8124" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="8125">
+      <c r="A8125" s="6" t="n">
+        <v>44882.583333333336</v>
+      </c>
+      <c r="B8125" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8125" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8126">
+      <c r="A8126" s="6" t="n">
+        <v>44882.59375</v>
+      </c>
+      <c r="B8126" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C8126" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8127">
+      <c r="A8127" s="6" t="n">
+        <v>44882.604166666664</v>
+      </c>
+      <c r="B8127" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8127" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8128">
+      <c r="A8128" s="6" t="n">
+        <v>44882.614583333336</v>
+      </c>
+      <c r="B8128" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8128" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="8129">
+      <c r="A8129" s="6" t="n">
+        <v>44882.625</v>
+      </c>
+      <c r="B8129" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C8129" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8130">
+      <c r="A8130" s="6" t="n">
+        <v>44882.635416666664</v>
+      </c>
+      <c r="B8130" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C8130" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8131">
+      <c r="A8131" s="6" t="n">
+        <v>44882.645833333336</v>
+      </c>
+      <c r="B8131" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C8131" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8132">
+      <c r="A8132" s="6" t="n">
+        <v>44882.65625</v>
+      </c>
+      <c r="B8132" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C8132" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8133">
+      <c r="A8133" s="6" t="n">
+        <v>44882.666666666664</v>
+      </c>
+      <c r="B8133" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C8133" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="8134">
+      <c r="A8134" s="6" t="n">
+        <v>44882.677083333336</v>
+      </c>
+      <c r="B8134" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C8134" s="1" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="8135">
+      <c r="A8135" s="6" t="n">
+        <v>44882.6875</v>
+      </c>
+      <c r="B8135" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8135" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8136">
+      <c r="A8136" s="6" t="n">
+        <v>44882.697916666664</v>
+      </c>
+      <c r="B8136" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C8136" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8137">
+      <c r="A8137" s="6" t="n">
+        <v>44882.708333333336</v>
+      </c>
+      <c r="B8137" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C8137" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8138">
+      <c r="A8138" s="6" t="n">
+        <v>44882.71875</v>
+      </c>
+      <c r="B8138" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8138" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="8139">
+      <c r="A8139" s="6" t="n">
+        <v>44882.729166666664</v>
+      </c>
+      <c r="B8139" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C8139" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8140">
+      <c r="A8140" s="6" t="n">
+        <v>44882.739583333336</v>
+      </c>
+      <c r="B8140" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C8140" s="1" t="n">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="8141">
+      <c r="A8141" s="6" t="n">
+        <v>44882.75</v>
+      </c>
+      <c r="B8141" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C8141" s="1" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="8142">
+      <c r="A8142" s="6" t="n">
+        <v>44882.760416666664</v>
+      </c>
+      <c r="B8142" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8142" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8143">
+      <c r="A8143" s="6" t="n">
+        <v>44882.770833333336</v>
+      </c>
+      <c r="B8143" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8143" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8144">
+      <c r="A8144" s="6" t="n">
+        <v>44882.78125</v>
+      </c>
+      <c r="B8144" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8144" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8145">
+      <c r="A8145" s="6" t="n">
+        <v>44882.791666666664</v>
+      </c>
+      <c r="B8145" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8145" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8146">
+      <c r="A8146" s="6" t="n">
+        <v>44882.802083333336</v>
+      </c>
+      <c r="B8146" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C8146" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8147">
+      <c r="A8147" s="6" t="n">
+        <v>44882.8125</v>
+      </c>
+      <c r="B8147" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C8147" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8148">
+      <c r="A8148" s="6" t="n">
+        <v>44882.822916666664</v>
+      </c>
+      <c r="B8148" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8148" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8149">
+      <c r="A8149" s="6" t="n">
+        <v>44882.833333333336</v>
+      </c>
+      <c r="B8149" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8149" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8150">
+      <c r="A8150" s="6" t="n">
+        <v>44882.84375</v>
+      </c>
+      <c r="B8150" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C8150" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8151">
+      <c r="A8151" s="6" t="n">
+        <v>44882.854166666664</v>
+      </c>
+      <c r="B8151" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8151" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8152">
+      <c r="A8152" s="6" t="n">
+        <v>44882.864583333336</v>
+      </c>
+      <c r="B8152" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8152" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8153">
+      <c r="A8153" s="6" t="n">
+        <v>44882.875</v>
+      </c>
+      <c r="B8153" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C8153" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8154">
+      <c r="A8154" s="6" t="n">
+        <v>44882.885416666664</v>
+      </c>
+      <c r="B8154" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8154" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8155">
+      <c r="A8155" s="6" t="n">
+        <v>44882.895833333336</v>
+      </c>
+      <c r="B8155" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8155" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8156">
+      <c r="A8156" s="6" t="n">
+        <v>44882.90625</v>
+      </c>
+      <c r="B8156" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8156" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8157">
+      <c r="A8157" s="6" t="n">
+        <v>44882.916666666664</v>
+      </c>
+      <c r="B8157" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8157" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8158">
+      <c r="A8158" s="6" t="n">
+        <v>44882.927083333336</v>
+      </c>
+      <c r="B8158" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8158" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8159">
+      <c r="A8159" s="6" t="n">
+        <v>44882.9375</v>
+      </c>
+      <c r="B8159" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8159" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8160">
+      <c r="A8160" s="6" t="n">
+        <v>44882.947916666664</v>
+      </c>
+      <c r="B8160" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8160" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8161">
+      <c r="A8161" s="6" t="n">
+        <v>44882.958333333336</v>
+      </c>
+      <c r="B8161" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8161" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8162">
+      <c r="A8162" s="6" t="n">
+        <v>44882.96875</v>
+      </c>
+      <c r="B8162" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8162" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8163">
+      <c r="A8163" s="6" t="n">
+        <v>44882.979166666664</v>
+      </c>
+      <c r="B8163" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C8163" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8164">
+      <c r="A8164" s="6" t="n">
+        <v>44882.989583333336</v>
+      </c>
+      <c r="B8164" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8164" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8165">
+      <c r="A8165" s="6" t="n">
+        <v>44883.0</v>
+      </c>
+      <c r="B8165" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8165" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8166">
+      <c r="A8166" s="6" t="n">
+        <v>44883.010416666664</v>
+      </c>
+      <c r="B8166" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8166" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8167">
+      <c r="A8167" s="6" t="n">
+        <v>44883.020833333336</v>
+      </c>
+      <c r="B8167" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8167" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8168">
+      <c r="A8168" s="6" t="n">
+        <v>44883.03125</v>
+      </c>
+      <c r="B8168" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8168" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8169">
+      <c r="A8169" s="6" t="n">
+        <v>44883.041666666664</v>
+      </c>
+      <c r="B8169" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8169" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8170">
+      <c r="A8170" s="6" t="n">
+        <v>44883.052083333336</v>
+      </c>
+      <c r="B8170" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8170" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8171">
+      <c r="A8171" s="6" t="n">
+        <v>44883.0625</v>
+      </c>
+      <c r="B8171" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8171" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8172">
+      <c r="A8172" s="6" t="n">
+        <v>44883.072916666664</v>
+      </c>
+      <c r="B8172" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8172" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8173">
+      <c r="A8173" s="6" t="n">
+        <v>44883.083333333336</v>
+      </c>
+      <c r="B8173" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8173" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8174">
+      <c r="A8174" s="6" t="n">
+        <v>44883.09375</v>
+      </c>
+      <c r="B8174" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8174" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8175">
+      <c r="A8175" s="6" t="n">
+        <v>44883.104166666664</v>
+      </c>
+      <c r="B8175" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8175" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8176">
+      <c r="A8176" s="6" t="n">
+        <v>44883.114583333336</v>
+      </c>
+      <c r="B8176" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8176" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8177">
+      <c r="A8177" s="6" t="n">
+        <v>44883.125</v>
+      </c>
+      <c r="B8177" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8177" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8178">
+      <c r="A8178" s="6" t="n">
+        <v>44883.135416666664</v>
+      </c>
+      <c r="B8178" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8178" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8179">
+      <c r="A8179" s="6" t="n">
+        <v>44883.145833333336</v>
+      </c>
+      <c r="B8179" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8179" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8180">
+      <c r="A8180" s="6" t="n">
+        <v>44883.15625</v>
+      </c>
+      <c r="B8180" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8180" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8181">
+      <c r="A8181" s="6" t="n">
+        <v>44883.166666666664</v>
+      </c>
+      <c r="B8181" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8181" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8182">
+      <c r="A8182" s="6" t="n">
+        <v>44883.177083333336</v>
+      </c>
+      <c r="B8182" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8182" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8183">
+      <c r="A8183" s="6" t="n">
+        <v>44883.1875</v>
+      </c>
+      <c r="B8183" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8183" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8184">
+      <c r="A8184" s="6" t="n">
+        <v>44883.197916666664</v>
+      </c>
+      <c r="B8184" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8184" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8185">
+      <c r="A8185" s="6" t="n">
+        <v>44883.208333333336</v>
+      </c>
+      <c r="B8185" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8185" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8186">
+      <c r="A8186" s="6" t="n">
+        <v>44883.21875</v>
+      </c>
+      <c r="B8186" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8186" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8187">
+      <c r="A8187" s="6" t="n">
+        <v>44883.229166666664</v>
+      </c>
+      <c r="B8187" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8187" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8188">
+      <c r="A8188" s="6" t="n">
+        <v>44883.239583333336</v>
+      </c>
+      <c r="B8188" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8188" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8189">
+      <c r="A8189" s="6" t="n">
+        <v>44883.25</v>
+      </c>
+      <c r="B8189" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8189" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8190">
+      <c r="A8190" s="6" t="n">
+        <v>44883.260416666664</v>
+      </c>
+      <c r="B8190" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8190" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8191">
+      <c r="A8191" s="6" t="n">
+        <v>44883.270833333336</v>
+      </c>
+      <c r="B8191" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8191" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8192">
+      <c r="A8192" s="6" t="n">
+        <v>44883.28125</v>
+      </c>
+      <c r="B8192" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8192" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8193">
+      <c r="A8193" s="6" t="n">
+        <v>44883.291666666664</v>
+      </c>
+      <c r="B8193" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8193" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8194">
+      <c r="A8194" s="6" t="n">
+        <v>44883.302083333336</v>
+      </c>
+      <c r="B8194" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8194" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8195">
+      <c r="A8195" s="6" t="n">
+        <v>44883.3125</v>
+      </c>
+      <c r="B8195" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8195" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8196">
+      <c r="A8196" s="6" t="n">
+        <v>44883.322916666664</v>
+      </c>
+      <c r="B8196" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C8196" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8197">
+      <c r="A8197" s="6" t="n">
+        <v>44883.333333333336</v>
+      </c>
+      <c r="B8197" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8197" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8198">
+      <c r="A8198" s="6" t="n">
+        <v>44883.34375</v>
+      </c>
+      <c r="B8198" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8198" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8199">
+      <c r="A8199" s="6" t="n">
+        <v>44883.354166666664</v>
+      </c>
+      <c r="B8199" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8199" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8200">
+      <c r="A8200" s="6" t="n">
+        <v>44883.364583333336</v>
+      </c>
+      <c r="B8200" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8200" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8201">
+      <c r="A8201" s="6" t="n">
+        <v>44883.375</v>
+      </c>
+      <c r="B8201" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8201" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8202">
+      <c r="A8202" s="6" t="n">
+        <v>44883.385416666664</v>
+      </c>
+      <c r="B8202" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8202" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8203">
+      <c r="A8203" s="6" t="n">
+        <v>44883.395833333336</v>
+      </c>
+      <c r="B8203" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8203" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8204">
+      <c r="A8204" s="6" t="n">
+        <v>44883.40625</v>
+      </c>
+      <c r="B8204" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8204" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8205">
+      <c r="A8205" s="6" t="n">
+        <v>44883.416666666664</v>
+      </c>
+      <c r="B8205" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8205" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8206">
+      <c r="A8206" s="6" t="n">
+        <v>44883.427083333336</v>
+      </c>
+      <c r="B8206" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8206" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8207">
+      <c r="A8207" s="6" t="n">
+        <v>44883.4375</v>
+      </c>
+      <c r="B8207" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8207" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8208">
+      <c r="A8208" s="6" t="n">
+        <v>44883.447916666664</v>
+      </c>
+      <c r="B8208" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8208" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8209">
+      <c r="A8209" s="6" t="n">
+        <v>44883.458333333336</v>
+      </c>
+      <c r="B8209" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8209" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8210">
+      <c r="A8210" s="6" t="n">
+        <v>44883.46875</v>
+      </c>
+      <c r="B8210" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8210" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8211">
+      <c r="A8211" s="6" t="n">
+        <v>44883.479166666664</v>
+      </c>
+      <c r="B8211" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8211" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8212">
+      <c r="A8212" s="6" t="n">
+        <v>44883.489583333336</v>
+      </c>
+      <c r="B8212" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8212" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8213">
+      <c r="A8213" s="6" t="n">
+        <v>44883.5</v>
+      </c>
+      <c r="B8213" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8213" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8214">
+      <c r="A8214" s="6" t="n">
+        <v>44883.510416666664</v>
+      </c>
+      <c r="B8214" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8214" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8215">
+      <c r="A8215" s="6" t="n">
+        <v>44883.520833333336</v>
+      </c>
+      <c r="B8215" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8215" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8216">
+      <c r="A8216" s="6" t="n">
+        <v>44883.53125</v>
+      </c>
+      <c r="B8216" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8216" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8217">
+      <c r="A8217" s="6" t="n">
+        <v>44883.541666666664</v>
+      </c>
+      <c r="B8217" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8217" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="8218">
+      <c r="A8218" s="6" t="n">
+        <v>44883.552083333336</v>
+      </c>
+      <c r="B8218" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8218" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8219">
+      <c r="A8219" s="6" t="n">
+        <v>44883.5625</v>
+      </c>
+      <c r="B8219" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8219" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8220">
+      <c r="A8220" s="6" t="n">
+        <v>44883.572916666664</v>
+      </c>
+      <c r="B8220" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8220" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8221">
+      <c r="A8221" s="6" t="n">
+        <v>44883.583333333336</v>
+      </c>
+      <c r="B8221" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8221" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8222">
+      <c r="A8222" s="6" t="n">
+        <v>44883.59375</v>
+      </c>
+      <c r="B8222" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8222" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8223">
+      <c r="A8223" s="6" t="n">
+        <v>44883.604166666664</v>
+      </c>
+      <c r="B8223" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8223" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8224">
+      <c r="A8224" s="6" t="n">
+        <v>44883.614583333336</v>
+      </c>
+      <c r="B8224" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8224" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8225">
+      <c r="A8225" s="6" t="n">
+        <v>44883.625</v>
+      </c>
+      <c r="B8225" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8225" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8226">
+      <c r="A8226" s="6" t="n">
+        <v>44883.635416666664</v>
+      </c>
+      <c r="B8226" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8226" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8227">
+      <c r="A8227" s="6" t="n">
+        <v>44883.645833333336</v>
+      </c>
+      <c r="B8227" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C8227" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8228">
+      <c r="A8228" s="6" t="n">
+        <v>44883.65625</v>
+      </c>
+      <c r="B8228" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C8228" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8229">
+      <c r="A8229" s="6" t="n">
+        <v>44883.666666666664</v>
+      </c>
+      <c r="B8229" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8229" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8230">
+      <c r="A8230" s="6" t="n">
+        <v>44883.677083333336</v>
+      </c>
+      <c r="B8230" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8230" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8231">
+      <c r="A8231" s="6" t="n">
+        <v>44883.6875</v>
+      </c>
+      <c r="B8231" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8231" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8232">
+      <c r="A8232" s="6" t="n">
+        <v>44883.697916666664</v>
+      </c>
+      <c r="B8232" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8232" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8233">
+      <c r="A8233" s="6" t="n">
+        <v>44883.708333333336</v>
+      </c>
+      <c r="B8233" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8233" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8234">
+      <c r="A8234" s="6" t="n">
+        <v>44883.71875</v>
+      </c>
+      <c r="B8234" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C8234" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8235">
+      <c r="A8235" s="6" t="n">
+        <v>44883.729166666664</v>
+      </c>
+      <c r="B8235" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C8235" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="8236">
+      <c r="A8236" s="6" t="n">
+        <v>44883.739583333336</v>
+      </c>
+      <c r="B8236" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8236" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="8237">
+      <c r="A8237" s="6" t="n">
+        <v>44883.75</v>
+      </c>
+      <c r="B8237" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8237" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8238">
+      <c r="A8238" s="6" t="n">
+        <v>44883.760416666664</v>
+      </c>
+      <c r="B8238" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8238" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8239">
+      <c r="A8239" s="6" t="n">
+        <v>44883.770833333336</v>
+      </c>
+      <c r="B8239" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8239" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8240">
+      <c r="A8240" s="6" t="n">
+        <v>44883.78125</v>
+      </c>
+      <c r="B8240" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8240" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8241">
+      <c r="A8241" s="6" t="n">
+        <v>44883.791666666664</v>
+      </c>
+      <c r="B8241" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8241" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8242">
+      <c r="A8242" s="6" t="n">
+        <v>44883.802083333336</v>
+      </c>
+      <c r="B8242" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8242" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8243">
+      <c r="A8243" s="6" t="n">
+        <v>44883.8125</v>
+      </c>
+      <c r="B8243" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8243" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8244">
+      <c r="A8244" s="6" t="n">
+        <v>44883.822916666664</v>
+      </c>
+      <c r="B8244" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8244" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8245">
+      <c r="A8245" s="6" t="n">
+        <v>44883.833333333336</v>
+      </c>
+      <c r="B8245" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8245" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8246">
+      <c r="A8246" s="6" t="n">
+        <v>44883.84375</v>
+      </c>
+      <c r="B8246" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8246" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8247">
+      <c r="A8247" s="6" t="n">
+        <v>44883.854166666664</v>
+      </c>
+      <c r="B8247" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8247" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8248">
+      <c r="A8248" s="6" t="n">
+        <v>44883.864583333336</v>
+      </c>
+      <c r="B8248" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8248" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8249">
+      <c r="A8249" s="6" t="n">
+        <v>44883.875</v>
+      </c>
+      <c r="B8249" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8249" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8250">
+      <c r="A8250" s="6" t="n">
+        <v>44883.885416666664</v>
+      </c>
+      <c r="B8250" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8250" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8251">
+      <c r="A8251" s="6" t="n">
+        <v>44883.895833333336</v>
+      </c>
+      <c r="B8251" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8251" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8252">
+      <c r="A8252" s="6" t="n">
+        <v>44883.90625</v>
+      </c>
+      <c r="B8252" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8252" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8253">
+      <c r="A8253" s="6" t="n">
+        <v>44883.916666666664</v>
+      </c>
+      <c r="B8253" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C8253" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8254">
+      <c r="A8254" s="6" t="n">
+        <v>44883.927083333336</v>
+      </c>
+      <c r="B8254" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8254" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8255">
+      <c r="A8255" s="6" t="n">
+        <v>44883.9375</v>
+      </c>
+      <c r="B8255" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8255" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8256">
+      <c r="A8256" s="6" t="n">
+        <v>44883.947916666664</v>
+      </c>
+      <c r="B8256" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8256" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8257">
+      <c r="A8257" s="6" t="n">
+        <v>44883.958333333336</v>
+      </c>
+      <c r="B8257" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8257" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8258">
+      <c r="A8258" s="6" t="n">
+        <v>44883.96875</v>
+      </c>
+      <c r="B8258" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8258" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8259">
+      <c r="A8259" s="6" t="n">
+        <v>44883.979166666664</v>
+      </c>
+      <c r="B8259" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8259" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8260">
+      <c r="A8260" s="6" t="n">
+        <v>44883.989583333336</v>
+      </c>
+      <c r="B8260" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8260" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8261">
+      <c r="A8261" s="6" t="n">
+        <v>44884.0</v>
+      </c>
+      <c r="B8261" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8261" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8262">
+      <c r="A8262" s="6" t="n">
+        <v>44884.010416666664</v>
+      </c>
+      <c r="B8262" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8262" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8263">
+      <c r="A8263" s="6" t="n">
+        <v>44884.020833333336</v>
+      </c>
+      <c r="B8263" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8263" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8264">
+      <c r="A8264" s="6" t="n">
+        <v>44884.03125</v>
+      </c>
+      <c r="B8264" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8264" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8265">
+      <c r="A8265" s="6" t="n">
+        <v>44884.041666666664</v>
+      </c>
+      <c r="B8265" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8265" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8266">
+      <c r="A8266" s="6" t="n">
+        <v>44884.052083333336</v>
+      </c>
+      <c r="B8266" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8266" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8267">
+      <c r="A8267" s="6" t="n">
+        <v>44884.0625</v>
+      </c>
+      <c r="B8267" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8267" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8268">
+      <c r="A8268" s="6" t="n">
+        <v>44884.072916666664</v>
+      </c>
+      <c r="B8268" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8268" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8269">
+      <c r="A8269" s="6" t="n">
+        <v>44884.083333333336</v>
+      </c>
+      <c r="B8269" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8269" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8270">
+      <c r="A8270" s="6" t="n">
+        <v>44884.09375</v>
+      </c>
+      <c r="B8270" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8270" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8271">
+      <c r="A8271" s="6" t="n">
+        <v>44884.104166666664</v>
+      </c>
+      <c r="B8271" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8271" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8272">
+      <c r="A8272" s="6" t="n">
+        <v>44884.114583333336</v>
+      </c>
+      <c r="B8272" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8272" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8273">
+      <c r="A8273" s="6" t="n">
+        <v>44884.125</v>
+      </c>
+      <c r="B8273" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8273" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8274">
+      <c r="A8274" s="6" t="n">
+        <v>44884.135416666664</v>
+      </c>
+      <c r="B8274" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8274" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8275">
+      <c r="A8275" s="6" t="n">
+        <v>44884.145833333336</v>
+      </c>
+      <c r="B8275" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8275" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8276">
+      <c r="A8276" s="6" t="n">
+        <v>44884.15625</v>
+      </c>
+      <c r="B8276" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8276" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8277">
+      <c r="A8277" s="6" t="n">
+        <v>44884.166666666664</v>
+      </c>
+      <c r="B8277" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8277" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8278">
+      <c r="A8278" s="6" t="n">
+        <v>44884.177083333336</v>
+      </c>
+      <c r="B8278" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8278" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8279">
+      <c r="A8279" s="6" t="n">
+        <v>44884.1875</v>
+      </c>
+      <c r="B8279" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8279" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8280">
+      <c r="A8280" s="6" t="n">
+        <v>44884.197916666664</v>
+      </c>
+      <c r="B8280" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8280" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8281">
+      <c r="A8281" s="6" t="n">
+        <v>44884.208333333336</v>
+      </c>
+      <c r="B8281" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8281" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8282">
+      <c r="A8282" s="6" t="n">
+        <v>44884.21875</v>
+      </c>
+      <c r="B8282" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8282" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8283">
+      <c r="A8283" s="6" t="n">
+        <v>44884.229166666664</v>
+      </c>
+      <c r="B8283" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8283" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8284">
+      <c r="A8284" s="6" t="n">
+        <v>44884.239583333336</v>
+      </c>
+      <c r="B8284" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8284" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8285">
+      <c r="A8285" s="6" t="n">
+        <v>44884.25</v>
+      </c>
+      <c r="B8285" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8285" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8286">
+      <c r="A8286" s="6" t="n">
+        <v>44884.260416666664</v>
+      </c>
+      <c r="B8286" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8286" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8287">
+      <c r="A8287" s="6" t="n">
+        <v>44884.270833333336</v>
+      </c>
+      <c r="B8287" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8287" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8288">
+      <c r="A8288" s="6" t="n">
+        <v>44884.28125</v>
+      </c>
+      <c r="B8288" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8288" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8289">
+      <c r="A8289" s="6" t="n">
+        <v>44884.291666666664</v>
+      </c>
+      <c r="B8289" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8289" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8290">
+      <c r="A8290" s="6" t="n">
+        <v>44884.302083333336</v>
+      </c>
+      <c r="B8290" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8290" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8291">
+      <c r="A8291" s="6" t="n">
+        <v>44884.3125</v>
+      </c>
+      <c r="B8291" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8291" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8292">
+      <c r="A8292" s="6" t="n">
+        <v>44884.322916666664</v>
+      </c>
+      <c r="B8292" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8292" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8293">
+      <c r="A8293" s="6" t="n">
+        <v>44884.333333333336</v>
+      </c>
+      <c r="B8293" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8293" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8294">
+      <c r="A8294" s="6" t="n">
+        <v>44884.34375</v>
+      </c>
+      <c r="B8294" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8294" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8295">
+      <c r="A8295" s="6" t="n">
+        <v>44884.354166666664</v>
+      </c>
+      <c r="B8295" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8295" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8296">
+      <c r="A8296" s="6" t="n">
+        <v>44884.364583333336</v>
+      </c>
+      <c r="B8296" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C8296" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8297">
+      <c r="A8297" s="6" t="n">
+        <v>44884.375</v>
+      </c>
+      <c r="B8297" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8297" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8298">
+      <c r="A8298" s="6" t="n">
+        <v>44884.385416666664</v>
+      </c>
+      <c r="B8298" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C8298" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8299">
+      <c r="A8299" s="6" t="n">
+        <v>44884.395833333336</v>
+      </c>
+      <c r="B8299" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8299" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="8300">
+      <c r="A8300" s="6" t="n">
+        <v>44884.40625</v>
+      </c>
+      <c r="B8300" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8300" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8301">
+      <c r="A8301" s="6" t="n">
+        <v>44884.416666666664</v>
+      </c>
+      <c r="B8301" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8301" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8302">
+      <c r="A8302" s="6" t="n">
+        <v>44884.427083333336</v>
+      </c>
+      <c r="B8302" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8302" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="8303">
+      <c r="A8303" s="6" t="n">
+        <v>44884.4375</v>
+      </c>
+      <c r="B8303" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8303" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8304">
+      <c r="A8304" s="6" t="n">
+        <v>44884.447916666664</v>
+      </c>
+      <c r="B8304" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8304" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8305">
+      <c r="A8305" s="6" t="n">
+        <v>44884.458333333336</v>
+      </c>
+      <c r="B8305" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8305" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8306">
+      <c r="A8306" s="6" t="n">
+        <v>44884.46875</v>
+      </c>
+      <c r="B8306" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8306" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8307">
+      <c r="A8307" s="6" t="n">
+        <v>44884.479166666664</v>
+      </c>
+      <c r="B8307" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8307" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8308">
+      <c r="A8308" s="6" t="n">
+        <v>44884.489583333336</v>
+      </c>
+      <c r="B8308" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8308" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8309">
+      <c r="A8309" s="6" t="n">
+        <v>44884.5</v>
+      </c>
+      <c r="B8309" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C8309" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8310">
+      <c r="A8310" s="6" t="n">
+        <v>44884.510416666664</v>
+      </c>
+      <c r="B8310" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8310" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8311">
+      <c r="A8311" s="6" t="n">
+        <v>44884.520833333336</v>
+      </c>
+      <c r="B8311" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8311" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8312">
+      <c r="A8312" s="6" t="n">
+        <v>44884.53125</v>
+      </c>
+      <c r="B8312" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8312" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="8313">
+      <c r="A8313" s="6" t="n">
+        <v>44884.541666666664</v>
+      </c>
+      <c r="B8313" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8313" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8314">
+      <c r="A8314" s="6" t="n">
+        <v>44884.552083333336</v>
+      </c>
+      <c r="B8314" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8314" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8315">
+      <c r="A8315" s="6" t="n">
+        <v>44884.5625</v>
+      </c>
+      <c r="B8315" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C8315" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8316">
+      <c r="A8316" s="6" t="n">
+        <v>44884.572916666664</v>
+      </c>
+      <c r="B8316" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8316" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8317">
+      <c r="A8317" s="6" t="n">
+        <v>44884.583333333336</v>
+      </c>
+      <c r="B8317" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C8317" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8318">
+      <c r="A8318" s="6" t="n">
+        <v>44884.59375</v>
+      </c>
+      <c r="B8318" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8318" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8319">
+      <c r="A8319" s="6" t="n">
+        <v>44884.604166666664</v>
+      </c>
+      <c r="B8319" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8319" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8320">
+      <c r="A8320" s="6" t="n">
+        <v>44884.614583333336</v>
+      </c>
+      <c r="B8320" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8320" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8321">
+      <c r="A8321" s="6" t="n">
+        <v>44884.625</v>
+      </c>
+      <c r="B8321" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8321" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8322">
+      <c r="A8322" s="6" t="n">
+        <v>44884.635416666664</v>
+      </c>
+      <c r="B8322" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8322" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8323">
+      <c r="A8323" s="6" t="n">
+        <v>44884.645833333336</v>
+      </c>
+      <c r="B8323" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8323" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8324">
+      <c r="A8324" s="6" t="n">
+        <v>44884.65625</v>
+      </c>
+      <c r="B8324" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C8324" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="8325">
+      <c r="A8325" s="6" t="n">
+        <v>44884.666666666664</v>
+      </c>
+      <c r="B8325" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C8325" s="1" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="8326">
+      <c r="A8326" s="6" t="n">
+        <v>44884.677083333336</v>
+      </c>
+      <c r="B8326" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C8326" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8327">
+      <c r="A8327" s="6" t="n">
+        <v>44884.6875</v>
+      </c>
+      <c r="B8327" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8327" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8328">
+      <c r="A8328" s="6" t="n">
+        <v>44884.697916666664</v>
+      </c>
+      <c r="B8328" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8328" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8329">
+      <c r="A8329" s="6" t="n">
+        <v>44884.708333333336</v>
+      </c>
+      <c r="B8329" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8329" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8330">
+      <c r="A8330" s="6" t="n">
+        <v>44884.71875</v>
+      </c>
+      <c r="B8330" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C8330" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8331">
+      <c r="A8331" s="6" t="n">
+        <v>44884.729166666664</v>
+      </c>
+      <c r="B8331" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8331" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8332">
+      <c r="A8332" s="6" t="n">
+        <v>44884.739583333336</v>
+      </c>
+      <c r="B8332" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8332" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8333">
+      <c r="A8333" s="6" t="n">
+        <v>44884.75</v>
+      </c>
+      <c r="B8333" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8333" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8334">
+      <c r="A8334" s="6" t="n">
+        <v>44884.760416666664</v>
+      </c>
+      <c r="B8334" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C8334" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8335">
+      <c r="A8335" s="6" t="n">
+        <v>44884.770833333336</v>
+      </c>
+      <c r="B8335" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8335" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8336">
+      <c r="A8336" s="6" t="n">
+        <v>44884.78125</v>
+      </c>
+      <c r="B8336" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8336" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8337">
+      <c r="A8337" s="6" t="n">
+        <v>44884.791666666664</v>
+      </c>
+      <c r="B8337" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8337" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8338">
+      <c r="A8338" s="6" t="n">
+        <v>44884.802083333336</v>
+      </c>
+      <c r="B8338" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8338" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8339">
+      <c r="A8339" s="6" t="n">
+        <v>44884.8125</v>
+      </c>
+      <c r="B8339" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8339" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8340">
+      <c r="A8340" s="6" t="n">
+        <v>44884.822916666664</v>
+      </c>
+      <c r="B8340" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8340" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8341">
+      <c r="A8341" s="6" t="n">
+        <v>44884.833333333336</v>
+      </c>
+      <c r="B8341" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8341" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8342">
+      <c r="A8342" s="6" t="n">
+        <v>44884.84375</v>
+      </c>
+      <c r="B8342" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8342" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8343">
+      <c r="A8343" s="6" t="n">
+        <v>44884.854166666664</v>
+      </c>
+      <c r="B8343" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8343" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8344">
+      <c r="A8344" s="6" t="n">
+        <v>44884.864583333336</v>
+      </c>
+      <c r="B8344" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8344" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8345">
+      <c r="A8345" s="6" t="n">
+        <v>44884.875</v>
+      </c>
+      <c r="B8345" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8345" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8346">
+      <c r="A8346" s="6" t="n">
+        <v>44884.885416666664</v>
+      </c>
+      <c r="B8346" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8346" s="1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8347">
+      <c r="A8347" s="6" t="n">
+        <v>44884.895833333336</v>
+      </c>
+      <c r="B8347" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8347" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8348">
+      <c r="A8348" s="6" t="n">
+        <v>44884.90625</v>
+      </c>
+      <c r="B8348" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8348" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8349">
+      <c r="A8349" s="6" t="n">
+        <v>44884.916666666664</v>
+      </c>
+      <c r="B8349" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8349" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8350">
+      <c r="A8350" s="6" t="n">
+        <v>44884.927083333336</v>
+      </c>
+      <c r="B8350" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8350" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8351">
+      <c r="A8351" s="6" t="n">
+        <v>44884.9375</v>
+      </c>
+      <c r="B8351" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8351" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8352">
+      <c r="A8352" s="6" t="n">
+        <v>44884.947916666664</v>
+      </c>
+      <c r="B8352" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8352" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8353">
+      <c r="A8353" s="6" t="n">
+        <v>44884.958333333336</v>
+      </c>
+      <c r="B8353" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C8353" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8354">
+      <c r="A8354" s="6" t="n">
+        <v>44884.96875</v>
+      </c>
+      <c r="B8354" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8354" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8355">
+      <c r="A8355" s="6" t="n">
+        <v>44884.979166666664</v>
+      </c>
+      <c r="B8355" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8355" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8356">
+      <c r="A8356" s="6" t="n">
+        <v>44884.989583333336</v>
+      </c>
+      <c r="B8356" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8356" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8357">
+      <c r="A8357" s="6" t="n">
+        <v>44885.0</v>
+      </c>
+      <c r="B8357" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8357" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8358">
+      <c r="A8358" s="6" t="n">
+        <v>44885.010416666664</v>
+      </c>
+      <c r="B8358" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8358" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8359">
+      <c r="A8359" s="6" t="n">
+        <v>44885.020833333336</v>
+      </c>
+      <c r="B8359" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8359" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8360">
+      <c r="A8360" s="6" t="n">
+        <v>44885.03125</v>
+      </c>
+      <c r="B8360" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8360" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8361">
+      <c r="A8361" s="6" t="n">
+        <v>44885.041666666664</v>
+      </c>
+      <c r="B8361" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8361" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8362">
+      <c r="A8362" s="6" t="n">
+        <v>44885.052083333336</v>
+      </c>
+      <c r="B8362" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8362" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8363">
+      <c r="A8363" s="6" t="n">
+        <v>44885.0625</v>
+      </c>
+      <c r="B8363" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8363" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8364">
+      <c r="A8364" s="6" t="n">
+        <v>44885.072916666664</v>
+      </c>
+      <c r="B8364" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8364" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8365">
+      <c r="A8365" s="6" t="n">
+        <v>44885.083333333336</v>
+      </c>
+      <c r="B8365" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8365" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8366">
+      <c r="A8366" s="6" t="n">
+        <v>44885.09375</v>
+      </c>
+      <c r="B8366" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8366" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8367">
+      <c r="A8367" s="6" t="n">
+        <v>44885.104166666664</v>
+      </c>
+      <c r="B8367" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8367" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8368">
+      <c r="A8368" s="6" t="n">
+        <v>44885.114583333336</v>
+      </c>
+      <c r="B8368" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8368" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8369">
+      <c r="A8369" s="6" t="n">
+        <v>44885.125</v>
+      </c>
+      <c r="B8369" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8369" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8370">
+      <c r="A8370" s="6" t="n">
+        <v>44885.135416666664</v>
+      </c>
+      <c r="B8370" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8370" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8371">
+      <c r="A8371" s="6" t="n">
+        <v>44885.145833333336</v>
+      </c>
+      <c r="B8371" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8371" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8372">
+      <c r="A8372" s="6" t="n">
+        <v>44885.15625</v>
+      </c>
+      <c r="B8372" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8372" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8373">
+      <c r="A8373" s="6" t="n">
+        <v>44885.166666666664</v>
+      </c>
+      <c r="B8373" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8373" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8374">
+      <c r="A8374" s="6" t="n">
+        <v>44885.177083333336</v>
+      </c>
+      <c r="B8374" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8374" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8375">
+      <c r="A8375" s="6" t="n">
+        <v>44885.1875</v>
+      </c>
+      <c r="B8375" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8375" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8376">
+      <c r="A8376" s="6" t="n">
+        <v>44885.197916666664</v>
+      </c>
+      <c r="B8376" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8376" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8377">
+      <c r="A8377" s="6" t="n">
+        <v>44885.208333333336</v>
+      </c>
+      <c r="B8377" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8377" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8378">
+      <c r="A8378" s="6" t="n">
+        <v>44885.21875</v>
+      </c>
+      <c r="B8378" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8378" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8379">
+      <c r="A8379" s="6" t="n">
+        <v>44885.229166666664</v>
+      </c>
+      <c r="B8379" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8379" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8380">
+      <c r="A8380" s="6" t="n">
+        <v>44885.239583333336</v>
+      </c>
+      <c r="B8380" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8380" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8381">
+      <c r="A8381" s="6" t="n">
+        <v>44885.25</v>
+      </c>
+      <c r="B8381" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8381" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8382">
+      <c r="A8382" s="6" t="n">
+        <v>44885.260416666664</v>
+      </c>
+      <c r="B8382" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8382" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8383">
+      <c r="A8383" s="6" t="n">
+        <v>44885.270833333336</v>
+      </c>
+      <c r="B8383" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8383" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8384">
+      <c r="A8384" s="6" t="n">
+        <v>44885.28125</v>
+      </c>
+      <c r="B8384" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8384" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8385">
+      <c r="A8385" s="6" t="n">
+        <v>44885.291666666664</v>
+      </c>
+      <c r="B8385" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8385" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8386">
+      <c r="A8386" s="6" t="n">
+        <v>44885.302083333336</v>
+      </c>
+      <c r="B8386" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8386" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8387">
+      <c r="A8387" s="6" t="n">
+        <v>44885.3125</v>
+      </c>
+      <c r="B8387" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8387" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8388">
+      <c r="A8388" s="6" t="n">
+        <v>44885.322916666664</v>
+      </c>
+      <c r="B8388" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8388" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8389">
+      <c r="A8389" s="6" t="n">
+        <v>44885.333333333336</v>
+      </c>
+      <c r="B8389" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8389" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8390">
+      <c r="A8390" s="6" t="n">
+        <v>44885.34375</v>
+      </c>
+      <c r="B8390" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8390" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8391">
+      <c r="A8391" s="6" t="n">
+        <v>44885.354166666664</v>
+      </c>
+      <c r="B8391" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8391" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8392">
+      <c r="A8392" s="6" t="n">
+        <v>44885.364583333336</v>
+      </c>
+      <c r="B8392" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8392" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8393">
+      <c r="A8393" s="6" t="n">
+        <v>44885.375</v>
+      </c>
+      <c r="B8393" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8393" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8394">
+      <c r="A8394" s="6" t="n">
+        <v>44885.385416666664</v>
+      </c>
+      <c r="B8394" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8394" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8395">
+      <c r="A8395" s="6" t="n">
+        <v>44885.395833333336</v>
+      </c>
+      <c r="B8395" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8395" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8396">
+      <c r="A8396" s="6" t="n">
+        <v>44885.40625</v>
+      </c>
+      <c r="B8396" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8396" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8397">
+      <c r="A8397" s="6" t="n">
+        <v>44885.416666666664</v>
+      </c>
+      <c r="B8397" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8397" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8398">
+      <c r="A8398" s="6" t="n">
+        <v>44885.427083333336</v>
+      </c>
+      <c r="B8398" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8398" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8399">
+      <c r="A8399" s="6" t="n">
+        <v>44885.4375</v>
+      </c>
+      <c r="B8399" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8399" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8400">
+      <c r="A8400" s="6" t="n">
+        <v>44885.447916666664</v>
+      </c>
+      <c r="B8400" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8400" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8401">
+      <c r="A8401" s="6" t="n">
+        <v>44885.458333333336</v>
+      </c>
+      <c r="B8401" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8401" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8402">
+      <c r="A8402" s="6" t="n">
+        <v>44885.46875</v>
+      </c>
+      <c r="B8402" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8402" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8403">
+      <c r="A8403" s="6" t="n">
+        <v>44885.479166666664</v>
+      </c>
+      <c r="B8403" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8403" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8404">
+      <c r="A8404" s="6" t="n">
+        <v>44885.489583333336</v>
+      </c>
+      <c r="B8404" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8404" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8405">
+      <c r="A8405" s="6" t="n">
+        <v>44885.5</v>
+      </c>
+      <c r="B8405" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8405" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8406">
+      <c r="A8406" s="6" t="n">
+        <v>44885.510416666664</v>
+      </c>
+      <c r="B8406" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8406" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8407">
+      <c r="A8407" s="6" t="n">
+        <v>44885.520833333336</v>
+      </c>
+      <c r="B8407" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8407" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8408">
+      <c r="A8408" s="6" t="n">
+        <v>44885.53125</v>
+      </c>
+      <c r="B8408" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8408" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8409">
+      <c r="A8409" s="6" t="n">
+        <v>44885.541666666664</v>
+      </c>
+      <c r="B8409" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8409" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8410">
+      <c r="A8410" s="6" t="n">
+        <v>44885.552083333336</v>
+      </c>
+      <c r="B8410" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8410" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8411">
+      <c r="A8411" s="6" t="n">
+        <v>44885.5625</v>
+      </c>
+      <c r="B8411" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8411" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8412">
+      <c r="A8412" s="6" t="n">
+        <v>44885.572916666664</v>
+      </c>
+      <c r="B8412" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8412" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8413">
+      <c r="A8413" s="6" t="n">
+        <v>44885.583333333336</v>
+      </c>
+      <c r="B8413" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8413" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8414">
+      <c r="A8414" s="6" t="n">
+        <v>44885.59375</v>
+      </c>
+      <c r="B8414" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8414" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8415">
+      <c r="A8415" s="6" t="n">
+        <v>44885.604166666664</v>
+      </c>
+      <c r="B8415" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8415" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8416">
+      <c r="A8416" s="6" t="n">
+        <v>44885.614583333336</v>
+      </c>
+      <c r="B8416" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8416" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8417">
+      <c r="A8417" s="6" t="n">
+        <v>44885.625</v>
+      </c>
+      <c r="B8417" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8417" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8418">
+      <c r="A8418" s="6" t="n">
+        <v>44885.635416666664</v>
+      </c>
+      <c r="B8418" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8418" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8419">
+      <c r="A8419" s="6" t="n">
+        <v>44885.645833333336</v>
+      </c>
+      <c r="B8419" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8419" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8420">
+      <c r="A8420" s="6" t="n">
+        <v>44885.65625</v>
+      </c>
+      <c r="B8420" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8420" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8421">
+      <c r="A8421" s="6" t="n">
+        <v>44885.666666666664</v>
+      </c>
+      <c r="B8421" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8421" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8422">
+      <c r="A8422" s="6" t="n">
+        <v>44885.677083333336</v>
+      </c>
+      <c r="B8422" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8422" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8423">
+      <c r="A8423" s="6" t="n">
+        <v>44885.6875</v>
+      </c>
+      <c r="B8423" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8423" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8424">
+      <c r="A8424" s="6" t="n">
+        <v>44885.697916666664</v>
+      </c>
+      <c r="B8424" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8424" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8425">
+      <c r="A8425" s="6" t="n">
+        <v>44885.708333333336</v>
+      </c>
+      <c r="B8425" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8425" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8426">
+      <c r="A8426" s="6" t="n">
+        <v>44885.71875</v>
+      </c>
+      <c r="B8426" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8426" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8427">
+      <c r="A8427" s="6" t="n">
+        <v>44885.729166666664</v>
+      </c>
+      <c r="B8427" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8427" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8428">
+      <c r="A8428" s="6" t="n">
+        <v>44885.739583333336</v>
+      </c>
+      <c r="B8428" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8428" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8429">
+      <c r="A8429" s="6" t="n">
+        <v>44885.75</v>
+      </c>
+      <c r="B8429" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8429" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8430">
+      <c r="A8430" s="6" t="n">
+        <v>44885.760416666664</v>
+      </c>
+      <c r="B8430" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8430" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8431">
+      <c r="A8431" s="6" t="n">
+        <v>44885.770833333336</v>
+      </c>
+      <c r="B8431" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8431" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8432">
+      <c r="A8432" s="6" t="n">
+        <v>44885.78125</v>
+      </c>
+      <c r="B8432" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8432" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8433">
+      <c r="A8433" s="6" t="n">
+        <v>44885.791666666664</v>
+      </c>
+      <c r="B8433" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8433" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8434">
+      <c r="A8434" s="6" t="n">
+        <v>44885.802083333336</v>
+      </c>
+      <c r="B8434" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8434" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8435">
+      <c r="A8435" s="6" t="n">
+        <v>44885.8125</v>
+      </c>
+      <c r="B8435" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8435" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8436">
+      <c r="A8436" s="6" t="n">
+        <v>44885.822916666664</v>
+      </c>
+      <c r="B8436" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8436" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8437">
+      <c r="A8437" s="6" t="n">
+        <v>44885.833333333336</v>
+      </c>
+      <c r="B8437" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8437" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8438">
+      <c r="A8438" s="6" t="n">
+        <v>44885.84375</v>
+      </c>
+      <c r="B8438" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8438" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8439">
+      <c r="A8439" s="6" t="n">
+        <v>44885.854166666664</v>
+      </c>
+      <c r="B8439" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8439" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8440">
+      <c r="A8440" s="6" t="n">
+        <v>44885.864583333336</v>
+      </c>
+      <c r="B8440" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8440" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8441">
+      <c r="A8441" s="6" t="n">
+        <v>44885.875</v>
+      </c>
+      <c r="B8441" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8441" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8442">
+      <c r="A8442" s="6" t="n">
+        <v>44885.885416666664</v>
+      </c>
+      <c r="B8442" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8442" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8443">
+      <c r="A8443" s="6" t="n">
+        <v>44885.895833333336</v>
+      </c>
+      <c r="B8443" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8443" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8444">
+      <c r="A8444" s="6" t="n">
+        <v>44885.90625</v>
+      </c>
+      <c r="B8444" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8444" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8445">
+      <c r="A8445" s="6" t="n">
+        <v>44885.916666666664</v>
+      </c>
+      <c r="B8445" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8445" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8446">
+      <c r="A8446" s="6" t="n">
+        <v>44885.927083333336</v>
+      </c>
+      <c r="B8446" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8446" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8447">
+      <c r="A8447" s="6" t="n">
+        <v>44885.9375</v>
+      </c>
+      <c r="B8447" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8447" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8448">
+      <c r="A8448" s="6" t="n">
+        <v>44885.947916666664</v>
+      </c>
+      <c r="B8448" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8448" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8449">
+      <c r="A8449" s="6" t="n">
+        <v>44885.958333333336</v>
+      </c>
+      <c r="B8449" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8449" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8450">
+      <c r="A8450" s="6" t="n">
+        <v>44885.96875</v>
+      </c>
+      <c r="B8450" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8450" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8451">
+      <c r="A8451" s="6" t="n">
+        <v>44885.979166666664</v>
+      </c>
+      <c r="B8451" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8451" s="1" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8452">
+      <c r="A8452" s="6" t="n">
+        <v>44885.989583333336</v>
+      </c>
+      <c r="B8452" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8452" s="1" t="n">
+        <v>0.0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>